<commit_message>
Modificações do 15 - 19
</commit_message>
<xml_diff>
--- a/Documentation/17-Analise_dos_Eventos_para_cada_Cenario.xlsx
+++ b/Documentation/17-Analise_dos_Eventos_para_cada_Cenario.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\re041584\OneDrive\Documentos\Impacta\Engenharia de Requisitos\Silpan\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/eed59d4ebf12600b/Documentos/Projeto/Faculdade/Silpan/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_F39CB75E9DCB1E95483200DF1B9D68301C93800A" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{773DB43D-9EFC-4644-B392-02C7212FFF55}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-9660" windowWidth="16440" windowHeight="38196"/>
+    <workbookView xWindow="-16320" yWindow="-8580" windowWidth="16440" windowHeight="38190" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DFD Orçamento sob medida" sheetId="5" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -164,9 +165,6 @@
     <t>x(6)</t>
   </si>
   <si>
-    <t>Criar pedido</t>
-  </si>
-  <si>
     <t>Cliente entrega orçamento</t>
   </si>
   <si>
@@ -195,12 +193,15 @@
   </si>
   <si>
     <t>Transportadora entrega pedido</t>
+  </si>
+  <si>
+    <t>Tratar pedido</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -648,48 +649,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -705,6 +664,48 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1020,38 +1021,38 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.88671875" customWidth="1"/>
-    <col min="4" max="4" width="52.33203125" customWidth="1"/>
-    <col min="5" max="5" width="12.5546875" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" customWidth="1"/>
+    <col min="4" max="4" width="52.28515625" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="34"/>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-    </row>
-    <row r="2" spans="1:10" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="36" t="s">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="20"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+    </row>
+    <row r="2" spans="1:10" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="37"/>
+      <c r="B2" s="23"/>
       <c r="C2" s="9" t="s">
         <v>1</v>
       </c>
@@ -1077,11 +1078,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="16.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3" s="38" t="s">
+    <row r="3" spans="1:10" ht="16.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="24" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="10">
@@ -1099,9 +1100,9 @@
       <c r="I3" s="4"/>
       <c r="J3" s="6"/>
     </row>
-    <row r="4" spans="1:10" ht="16.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="21"/>
-      <c r="B4" s="39"/>
+    <row r="4" spans="1:10" ht="16.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="28"/>
+      <c r="B4" s="25"/>
       <c r="C4" s="11">
         <f>C3+1</f>
         <v>2</v>
@@ -1118,9 +1119,9 @@
       <c r="I4" s="4"/>
       <c r="J4" s="6"/>
     </row>
-    <row r="5" spans="1:10" ht="16.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="21"/>
-      <c r="B5" s="39"/>
+    <row r="5" spans="1:10" ht="16.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="28"/>
+      <c r="B5" s="25"/>
       <c r="C5" s="11">
         <f t="shared" ref="C5:C8" si="0">C4+1</f>
         <v>3</v>
@@ -1137,9 +1138,9 @@
       <c r="I5" s="4"/>
       <c r="J5" s="6"/>
     </row>
-    <row r="6" spans="1:10" ht="16.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="21"/>
-      <c r="B6" s="39"/>
+    <row r="6" spans="1:10" ht="16.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="28"/>
+      <c r="B6" s="25"/>
       <c r="C6" s="11">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1156,9 +1157,9 @@
       <c r="I6" s="4"/>
       <c r="J6" s="6"/>
     </row>
-    <row r="7" spans="1:10" ht="16.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="21"/>
-      <c r="B7" s="39"/>
+    <row r="7" spans="1:10" ht="16.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="28"/>
+      <c r="B7" s="25"/>
       <c r="C7" s="11">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1175,9 +1176,9 @@
       <c r="I7" s="4"/>
       <c r="J7" s="6"/>
     </row>
-    <row r="8" spans="1:10" ht="16.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="22"/>
-      <c r="B8" s="40"/>
+    <row r="8" spans="1:10" ht="16.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="29"/>
+      <c r="B8" s="26"/>
       <c r="C8" s="11">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1194,11 +1195,11 @@
       <c r="I8" s="4"/>
       <c r="J8" s="6"/>
     </row>
-    <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="26" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9" s="30" t="s">
+    <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="34" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="12">
@@ -1216,9 +1217,9 @@
       <c r="I9" s="15"/>
       <c r="J9" s="16"/>
     </row>
-    <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="27"/>
-      <c r="B10" s="31"/>
+    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="31"/>
+      <c r="B10" s="35"/>
       <c r="C10" s="7">
         <f>C9+1</f>
         <v>2</v>
@@ -1235,9 +1236,9 @@
       <c r="I10" s="4"/>
       <c r="J10" s="6"/>
     </row>
-    <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="27"/>
-      <c r="B11" s="31"/>
+    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="31"/>
+      <c r="B11" s="35"/>
       <c r="C11" s="7">
         <f>C10+1</f>
         <v>3</v>
@@ -1254,9 +1255,9 @@
       <c r="I11" s="4"/>
       <c r="J11" s="6"/>
     </row>
-    <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="27"/>
-      <c r="B12" s="31"/>
+    <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="31"/>
+      <c r="B12" s="35"/>
       <c r="C12" s="7">
         <f>C11+1</f>
         <v>4</v>
@@ -1273,9 +1274,9 @@
       <c r="I12" s="4"/>
       <c r="J12" s="6"/>
     </row>
-    <row r="13" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="28"/>
-      <c r="B13" s="32" t="s">
+    <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="32"/>
+      <c r="B13" s="36" t="s">
         <v>26</v>
       </c>
       <c r="C13" s="7">
@@ -1294,9 +1295,9 @@
       </c>
       <c r="J13" s="16"/>
     </row>
-    <row r="14" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="29"/>
-      <c r="B14" s="33"/>
+    <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="33"/>
+      <c r="B14" s="37"/>
       <c r="C14" s="7">
         <f t="shared" si="1"/>
         <v>6</v>
@@ -1313,18 +1314,18 @@
       <c r="I14" s="4"/>
       <c r="J14" s="6"/>
     </row>
-    <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" s="23" t="s">
+    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="38" t="s">
         <v>9</v>
       </c>
       <c r="C15" s="7">
         <v>1</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="5" t="s">
@@ -1335,9 +1336,9 @@
       <c r="I15" s="4"/>
       <c r="J15" s="6"/>
     </row>
-    <row r="16" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="21"/>
-      <c r="B16" s="24"/>
+    <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="28"/>
+      <c r="B16" s="39"/>
       <c r="C16" s="7">
         <f t="shared" ref="C16:C23" si="2">C15+1</f>
         <v>2</v>
@@ -1354,15 +1355,15 @@
       <c r="I16" s="4"/>
       <c r="J16" s="6"/>
     </row>
-    <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="21"/>
-      <c r="B17" s="24"/>
+    <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="28"/>
+      <c r="B17" s="39"/>
       <c r="C17" s="7">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
@@ -1373,15 +1374,15 @@
       <c r="I17" s="4"/>
       <c r="J17" s="6"/>
     </row>
-    <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="21"/>
-      <c r="B18" s="24"/>
+    <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="28"/>
+      <c r="B18" s="39"/>
       <c r="C18" s="7">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>17</v>
@@ -1392,15 +1393,15 @@
       <c r="I18" s="4"/>
       <c r="J18" s="6"/>
     </row>
-    <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="21"/>
-      <c r="B19" s="24"/>
+    <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="28"/>
+      <c r="B19" s="39"/>
       <c r="C19" s="7">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>19</v>
@@ -1411,15 +1412,15 @@
       <c r="I19" s="4"/>
       <c r="J19" s="6"/>
     </row>
-    <row r="20" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="21"/>
-      <c r="B20" s="24"/>
+    <row r="20" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="28"/>
+      <c r="B20" s="39"/>
       <c r="C20" s="7">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>21</v>
@@ -1430,15 +1431,15 @@
       <c r="I20" s="4"/>
       <c r="J20" s="6"/>
     </row>
-    <row r="21" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="21"/>
-      <c r="B21" s="24"/>
+    <row r="21" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="28"/>
+      <c r="B21" s="39"/>
       <c r="C21" s="7">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>29</v>
@@ -1449,27 +1450,27 @@
       <c r="I21" s="4"/>
       <c r="J21" s="6"/>
     </row>
-    <row r="22" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="21"/>
-      <c r="B22" s="25"/>
+    <row r="22" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="28"/>
+      <c r="B22" s="40"/>
       <c r="C22" s="7">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="D22" s="18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
       <c r="G22" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
       <c r="J22" s="6"/>
     </row>
-    <row r="23" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="22"/>
+    <row r="23" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="29"/>
       <c r="B23" s="19" t="s">
         <v>26</v>
       </c>
@@ -1491,6 +1492,8 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A15:A23"/>
+    <mergeCell ref="B15:B22"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="B3:B8"/>
@@ -1498,8 +1501,6 @@
     <mergeCell ref="A9:A14"/>
     <mergeCell ref="B9:B12"/>
     <mergeCell ref="B13:B14"/>
-    <mergeCell ref="A15:A23"/>
-    <mergeCell ref="B15:B22"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Modificações no art. 15 - 18, rev. art 15 - 17
</commit_message>
<xml_diff>
--- a/Documentation/17-Analise_dos_Eventos_para_cada_Cenario.xlsx
+++ b/Documentation/17-Analise_dos_Eventos_para_cada_Cenario.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/eed59d4ebf12600b/Documentos/Projeto/Faculdade/Silpan/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_F39CB75E9DCB1E95483200DF1B9D68301C93800A" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{773DB43D-9EFC-4644-B392-02C7212FFF55}"/>
+  <xr:revisionPtr revIDLastSave="51" documentId="11_F39CB75E9DCB1E95483200DF1B9D68301C93800A" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{944040FC-F9E1-43D5-9A17-76ECFC02BFC3}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-8580" windowWidth="16440" windowHeight="38190" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DFD Orçamento sob medida" sheetId="5" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="52">
   <si>
     <t>Capacidades</t>
   </si>
@@ -150,9 +150,6 @@
     <t>Vendedor analisa solicitação</t>
   </si>
   <si>
-    <t>Consultor gera orçamento</t>
-  </si>
-  <si>
     <t>FA</t>
   </si>
   <si>
@@ -162,18 +159,12 @@
     <t>Fabricante envia orçamento</t>
   </si>
   <si>
-    <t>x(6)</t>
-  </si>
-  <si>
     <t>Cliente entrega orçamento</t>
   </si>
   <si>
     <t>vendedor efetiva o pedido</t>
   </si>
   <si>
-    <t>Cliente efetua pagamento</t>
-  </si>
-  <si>
     <t>Almoxarife verifica estoque</t>
   </si>
   <si>
@@ -192,17 +183,59 @@
     <t xml:space="preserve">Tratar orçamento </t>
   </si>
   <si>
-    <t>Transportadora entrega pedido</t>
-  </si>
-  <si>
     <t>Tratar pedido</t>
+  </si>
+  <si>
+    <t>Cliente efetua pagamento em dinheiro</t>
+  </si>
+  <si>
+    <t>x(8)</t>
+  </si>
+  <si>
+    <t>x(9)</t>
+  </si>
+  <si>
+    <t>x(10)</t>
+  </si>
+  <si>
+    <t>x(11)</t>
+  </si>
+  <si>
+    <t>x(6, 10)</t>
+  </si>
+  <si>
+    <t>x(13)</t>
+  </si>
+  <si>
+    <t>x(15)</t>
+  </si>
+  <si>
+    <t>x(16, 17)</t>
+  </si>
+  <si>
+    <t>x(18)</t>
+  </si>
+  <si>
+    <t>x(19)</t>
+  </si>
+  <si>
+    <t>Vendedor entrega pedido</t>
+  </si>
+  <si>
+    <t>x(20)</t>
+  </si>
+  <si>
+    <t>x(14,22)</t>
+  </si>
+  <si>
+    <t>Cliente efetua pagamento cartão ou Pix</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -249,6 +282,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -611,9 +658,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -626,9 +670,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -648,6 +689,28 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -666,15 +729,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -697,15 +751,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1022,10 +1067,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1037,23 +1082,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="20"/>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
+      <c r="A1" s="26"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
     </row>
     <row r="2" spans="1:10" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="9" t="s">
+      <c r="B2" s="29"/>
+      <c r="C2" s="8" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -1079,16 +1124,16 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="16.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="B3" s="24" t="s">
+      <c r="A3" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="9">
         <v>1</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="7" t="s">
         <v>10</v>
       </c>
       <c r="E3" s="5"/>
@@ -1101,13 +1146,13 @@
       <c r="J3" s="6"/>
     </row>
     <row r="4" spans="1:10" ht="16.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="28"/>
-      <c r="B4" s="25"/>
-      <c r="C4" s="11">
+      <c r="A4" s="21"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="10">
         <f>C3+1</f>
         <v>2</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="7" t="s">
         <v>12</v>
       </c>
       <c r="E4" s="5"/>
@@ -1120,13 +1165,13 @@
       <c r="J4" s="6"/>
     </row>
     <row r="5" spans="1:10" ht="16.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="28"/>
-      <c r="B5" s="25"/>
-      <c r="C5" s="11">
-        <f t="shared" ref="C5:C8" si="0">C4+1</f>
+      <c r="A5" s="21"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="10">
+        <f t="shared" ref="C5:C24" si="0">C4+1</f>
         <v>3</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="7" t="s">
         <v>14</v>
       </c>
       <c r="E5" s="5" t="s">
@@ -1139,13 +1184,13 @@
       <c r="J5" s="6"/>
     </row>
     <row r="6" spans="1:10" ht="16.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="28"/>
-      <c r="B6" s="25"/>
-      <c r="C6" s="11">
+      <c r="A6" s="21"/>
+      <c r="B6" s="31"/>
+      <c r="C6" s="10">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="7" t="s">
         <v>16</v>
       </c>
       <c r="E6" s="5"/>
@@ -1158,13 +1203,13 @@
       <c r="J6" s="6"/>
     </row>
     <row r="7" spans="1:10" ht="16.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="28"/>
-      <c r="B7" s="25"/>
-      <c r="C7" s="11">
+      <c r="A7" s="21"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="10">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="7" t="s">
         <v>18</v>
       </c>
       <c r="E7" s="5" t="s">
@@ -1177,13 +1222,13 @@
       <c r="J7" s="6"/>
     </row>
     <row r="8" spans="1:10" ht="16.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="29"/>
-      <c r="B8" s="26"/>
-      <c r="C8" s="11">
+      <c r="A8" s="22"/>
+      <c r="B8" s="32"/>
+      <c r="C8" s="10">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="7" t="s">
         <v>20</v>
       </c>
       <c r="E8" s="5"/>
@@ -1196,39 +1241,40 @@
       <c r="J8" s="6"/>
     </row>
     <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="B9" s="34" t="s">
+      <c r="A9" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="12">
-        <v>1</v>
-      </c>
-      <c r="D9" s="13" t="s">
+      <c r="C9" s="10">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="D9" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14" t="s">
+      <c r="E9" s="12"/>
+      <c r="F9" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="16"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="14"/>
     </row>
     <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="31"/>
-      <c r="B10" s="35"/>
-      <c r="C10" s="7">
-        <f>C9+1</f>
-        <v>2</v>
-      </c>
-      <c r="D10" s="8" t="s">
+      <c r="A10" s="34"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="10">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="D10" s="7" t="s">
         <v>23</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="F10" s="5"/>
       <c r="G10" s="4"/>
@@ -1237,76 +1283,76 @@
       <c r="J10" s="6"/>
     </row>
     <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="31"/>
-      <c r="B11" s="35"/>
-      <c r="C11" s="7">
-        <f>C10+1</f>
-        <v>3</v>
-      </c>
-      <c r="D11" s="8" t="s">
+      <c r="A11" s="34"/>
+      <c r="B11" s="38"/>
+      <c r="C11" s="10">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="D11" s="7" t="s">
         <v>24</v>
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
       <c r="G11" s="4" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
       <c r="J11" s="6"/>
     </row>
     <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="31"/>
-      <c r="B12" s="35"/>
-      <c r="C12" s="7">
-        <f>C11+1</f>
-        <v>4</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>25</v>
+      <c r="A12" s="34"/>
+      <c r="B12" s="38"/>
+      <c r="C12" s="10">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>20</v>
       </c>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
       <c r="G12" s="4" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
       <c r="J12" s="6"/>
     </row>
     <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="32"/>
-      <c r="B13" s="36" t="s">
+      <c r="A13" s="35"/>
+      <c r="B13" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="10">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="D13" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="7">
-        <f t="shared" ref="C13:C14" si="1">C12+1</f>
-        <v>5</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
-      <c r="I13" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="J13" s="16"/>
+      <c r="I13" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="J13" s="14"/>
     </row>
     <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="33"/>
-      <c r="B14" s="37"/>
-      <c r="C14" s="7">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>28</v>
+      <c r="A14" s="36"/>
+      <c r="B14" s="40"/>
+      <c r="C14" s="10">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>27</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="F14" s="5"/>
       <c r="G14" s="4"/>
@@ -1315,21 +1361,22 @@
       <c r="J14" s="6"/>
     </row>
     <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="B15" s="38" t="s">
+      <c r="A15" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="7">
-        <v>1</v>
+      <c r="C15" s="10">
+        <f t="shared" si="0"/>
+        <v>13</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="5" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
@@ -1337,11 +1384,11 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="28"/>
-      <c r="B16" s="39"/>
-      <c r="C16" s="7">
-        <f t="shared" ref="C16:C23" si="2">C15+1</f>
-        <v>2</v>
+      <c r="A16" s="21"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="10">
+        <f>C15+1</f>
+        <v>14</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>12</v>
@@ -1349,43 +1396,43 @@
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
       <c r="G16" s="4" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
       <c r="J16" s="6"/>
     </row>
     <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="28"/>
-      <c r="B17" s="39"/>
-      <c r="C17" s="7">
-        <f t="shared" si="2"/>
-        <v>3</v>
+      <c r="A17" s="21"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="10">
+        <f t="shared" si="0"/>
+        <v>15</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="4" t="s">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
       <c r="J17" s="6"/>
     </row>
     <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="28"/>
-      <c r="B18" s="39"/>
-      <c r="C18" s="7">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>32</v>
+      <c r="A18" s="21"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="10">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>37</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>17</v>
+        <v>44</v>
       </c>
       <c r="F18" s="5"/>
       <c r="G18" s="4"/>
@@ -1394,17 +1441,17 @@
       <c r="J18" s="6"/>
     </row>
     <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="28"/>
-      <c r="B19" s="39"/>
-      <c r="C19" s="7">
-        <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>33</v>
+      <c r="A19" s="21"/>
+      <c r="B19" s="24"/>
+      <c r="C19" s="10">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>51</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="F19" s="5"/>
       <c r="G19" s="4"/>
@@ -1413,17 +1460,17 @@
       <c r="J19" s="6"/>
     </row>
     <row r="20" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="28"/>
-      <c r="B20" s="39"/>
-      <c r="C20" s="7">
-        <f t="shared" si="2"/>
-        <v>6</v>
+      <c r="A20" s="21"/>
+      <c r="B20" s="24"/>
+      <c r="C20" s="10">
+        <f t="shared" si="0"/>
+        <v>18</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="F20" s="5"/>
       <c r="G20" s="4"/>
@@ -1432,17 +1479,17 @@
       <c r="J20" s="6"/>
     </row>
     <row r="21" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="28"/>
-      <c r="B21" s="39"/>
-      <c r="C21" s="7">
-        <f t="shared" si="2"/>
-        <v>7</v>
+      <c r="A21" s="21"/>
+      <c r="B21" s="24"/>
+      <c r="C21" s="10">
+        <f t="shared" si="0"/>
+        <v>19</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="F21" s="5"/>
       <c r="G21" s="4"/>
@@ -1451,49 +1498,71 @@
       <c r="J21" s="6"/>
     </row>
     <row r="22" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="28"/>
-      <c r="B22" s="40"/>
-      <c r="C22" s="7">
-        <f t="shared" si="2"/>
-        <v>8</v>
-      </c>
-      <c r="D22" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="E22" s="5"/>
+      <c r="A22" s="21"/>
+      <c r="B22" s="24"/>
+      <c r="C22" s="10">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>47</v>
+      </c>
       <c r="F22" s="5"/>
-      <c r="G22" s="4" t="s">
-        <v>36</v>
-      </c>
+      <c r="G22" s="4"/>
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
       <c r="J22" s="6"/>
     </row>
     <row r="23" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="29"/>
-      <c r="B23" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="C23" s="7">
-        <f t="shared" si="2"/>
-        <v>9</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>22</v>
+      <c r="A23" s="21"/>
+      <c r="B23" s="25"/>
+      <c r="C23" s="10">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="D23" s="16" t="s">
+        <v>48</v>
       </c>
       <c r="E23" s="5"/>
-      <c r="F23" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G23" s="4"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="4" t="s">
+        <v>49</v>
+      </c>
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
       <c r="J23" s="6"/>
     </row>
+    <row r="24" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="22"/>
+      <c r="B24" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="10">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="6"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D28" s="19"/>
+    </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="A15:A23"/>
-    <mergeCell ref="B15:B22"/>
+    <mergeCell ref="A15:A24"/>
+    <mergeCell ref="B15:B23"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="B3:B8"/>

</xml_diff>

<commit_message>
rev. 15 - 19 completa
</commit_message>
<xml_diff>
--- a/Documentation/17-Analise_dos_Eventos_para_cada_Cenario.xlsx
+++ b/Documentation/17-Analise_dos_Eventos_para_cada_Cenario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/eed59d4ebf12600b/Documentos/Projeto/Faculdade/Silpan/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="51" documentId="11_F39CB75E9DCB1E95483200DF1B9D68301C93800A" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{944040FC-F9E1-43D5-9A17-76ECFC02BFC3}"/>
+  <xr:revisionPtr revIDLastSave="84" documentId="11_F39CB75E9DCB1E95483200DF1B9D68301C93800A" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{EED2EF43-0E5A-4B72-BEAB-719CF1BB692C}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="54">
   <si>
     <t>Capacidades</t>
   </si>
@@ -162,9 +162,6 @@
     <t>Cliente entrega orçamento</t>
   </si>
   <si>
-    <t>vendedor efetiva o pedido</t>
-  </si>
-  <si>
     <t>Almoxarife verifica estoque</t>
   </si>
   <si>
@@ -207,9 +204,6 @@
     <t>x(13)</t>
   </si>
   <si>
-    <t>x(15)</t>
-  </si>
-  <si>
     <t>x(16, 17)</t>
   </si>
   <si>
@@ -225,10 +219,22 @@
     <t>x(20)</t>
   </si>
   <si>
-    <t>x(14,22)</t>
-  </si>
-  <si>
     <t>Cliente efetua pagamento cartão ou Pix</t>
+  </si>
+  <si>
+    <t>x(22)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vendedor recebe pedido do cliente  </t>
+  </si>
+  <si>
+    <t>Vendedor efetiva pedido com orçamento</t>
+  </si>
+  <si>
+    <t>x(14)</t>
+  </si>
+  <si>
+    <t>x(15, 23)</t>
   </si>
 </sst>
 </file>
@@ -531,7 +537,39 @@
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
-      <right/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
       <top/>
       <bottom style="medium">
         <color rgb="FF000000"/>
@@ -545,6 +583,15 @@
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
@@ -554,82 +601,43 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </left>
       <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
       </top>
       <bottom style="medium">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="medium">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </right>
       <top style="medium">
         <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
@@ -637,7 +645,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -672,23 +680,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -701,15 +706,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -732,26 +728,41 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1069,8 +1080,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1082,22 +1093,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="26"/>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
+      <c r="A1" s="22"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
     </row>
     <row r="2" spans="1:10" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="29"/>
+      <c r="B2" s="25"/>
       <c r="C2" s="8" t="s">
         <v>1</v>
       </c>
@@ -1124,10 +1135,10 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="16.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="B3" s="30" t="s">
+      <c r="A3" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="26" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="9">
@@ -1146,8 +1157,8 @@
       <c r="J3" s="6"/>
     </row>
     <row r="4" spans="1:10" ht="16.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="21"/>
-      <c r="B4" s="31"/>
+      <c r="A4" s="20"/>
+      <c r="B4" s="27"/>
       <c r="C4" s="10">
         <f>C3+1</f>
         <v>2</v>
@@ -1165,10 +1176,10 @@
       <c r="J4" s="6"/>
     </row>
     <row r="5" spans="1:10" ht="16.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="21"/>
-      <c r="B5" s="31"/>
+      <c r="A5" s="20"/>
+      <c r="B5" s="27"/>
       <c r="C5" s="10">
-        <f t="shared" ref="C5:C24" si="0">C4+1</f>
+        <f t="shared" ref="C5:C25" si="0">C4+1</f>
         <v>3</v>
       </c>
       <c r="D5" s="7" t="s">
@@ -1184,8 +1195,8 @@
       <c r="J5" s="6"/>
     </row>
     <row r="6" spans="1:10" ht="16.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="21"/>
-      <c r="B6" s="31"/>
+      <c r="A6" s="20"/>
+      <c r="B6" s="27"/>
       <c r="C6" s="10">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1203,8 +1214,8 @@
       <c r="J6" s="6"/>
     </row>
     <row r="7" spans="1:10" ht="16.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="21"/>
-      <c r="B7" s="31"/>
+      <c r="A7" s="20"/>
+      <c r="B7" s="27"/>
       <c r="C7" s="10">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1222,8 +1233,8 @@
       <c r="J7" s="6"/>
     </row>
     <row r="8" spans="1:10" ht="16.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="22"/>
-      <c r="B8" s="32"/>
+      <c r="A8" s="21"/>
+      <c r="B8" s="28"/>
       <c r="C8" s="10">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1241,10 +1252,10 @@
       <c r="J8" s="6"/>
     </row>
     <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="33" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9" s="37" t="s">
+      <c r="A9" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="32" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="10">
@@ -1264,8 +1275,8 @@
       <c r="J9" s="14"/>
     </row>
     <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="34"/>
-      <c r="B10" s="38"/>
+      <c r="A10" s="30"/>
+      <c r="B10" s="33"/>
       <c r="C10" s="10">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1274,7 +1285,7 @@
         <v>23</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F10" s="5"/>
       <c r="G10" s="4"/>
@@ -1283,8 +1294,8 @@
       <c r="J10" s="6"/>
     </row>
     <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="34"/>
-      <c r="B11" s="38"/>
+      <c r="A11" s="30"/>
+      <c r="B11" s="33"/>
       <c r="C11" s="10">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1295,15 +1306,15 @@
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
       <c r="G11" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
       <c r="J11" s="6"/>
     </row>
     <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="34"/>
-      <c r="B12" s="38"/>
+      <c r="A12" s="30"/>
+      <c r="B12" s="33"/>
       <c r="C12" s="10">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1314,15 +1325,15 @@
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
       <c r="G12" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
       <c r="J12" s="6"/>
     </row>
     <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="35"/>
-      <c r="B13" s="39" t="s">
+      <c r="A13" s="31"/>
+      <c r="B13" s="34" t="s">
         <v>25</v>
       </c>
       <c r="C13" s="10">
@@ -1337,13 +1348,13 @@
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
       <c r="I13" s="15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J13" s="14"/>
     </row>
     <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="36"/>
-      <c r="B14" s="40"/>
+      <c r="A14" s="31"/>
+      <c r="B14" s="35"/>
       <c r="C14" s="10">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1352,7 +1363,7 @@
         <v>27</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F14" s="5"/>
       <c r="G14" s="4"/>
@@ -1360,11 +1371,11 @@
       <c r="I14" s="4"/>
       <c r="J14" s="6"/>
     </row>
-    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" s="23" t="s">
+    <row r="15" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="26" t="s">
         <v>9</v>
       </c>
       <c r="C15" s="10">
@@ -1374,18 +1385,18 @@
       <c r="D15" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5" t="s">
-        <v>42</v>
-      </c>
+      <c r="E15" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" s="5"/>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="21"/>
-      <c r="B16" s="24"/>
+      <c r="A16" s="20"/>
+      <c r="B16" s="27"/>
       <c r="C16" s="10">
         <f>C15+1</f>
         <v>14</v>
@@ -1396,43 +1407,43 @@
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
       <c r="G16" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
       <c r="J16" s="6"/>
     </row>
     <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="21"/>
-      <c r="B17" s="24"/>
+      <c r="A17" s="20"/>
+      <c r="B17" s="27"/>
       <c r="C17" s="10">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="4" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
       <c r="J17" s="6"/>
     </row>
     <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="21"/>
-      <c r="B18" s="24"/>
+      <c r="A18" s="20"/>
+      <c r="B18" s="27"/>
       <c r="C18" s="10">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="D18" s="18" t="s">
-        <v>37</v>
+      <c r="D18" s="17" t="s">
+        <v>36</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="F18" s="5"/>
       <c r="G18" s="4"/>
@@ -1441,17 +1452,17 @@
       <c r="J18" s="6"/>
     </row>
     <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="21"/>
-      <c r="B19" s="24"/>
+      <c r="A19" s="20"/>
+      <c r="B19" s="27"/>
       <c r="C19" s="10">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="D19" s="18" t="s">
-        <v>51</v>
+      <c r="D19" s="17" t="s">
+        <v>48</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="F19" s="5"/>
       <c r="G19" s="4"/>
@@ -1460,17 +1471,17 @@
       <c r="J19" s="6"/>
     </row>
     <row r="20" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="21"/>
-      <c r="B20" s="24"/>
+      <c r="A20" s="20"/>
+      <c r="B20" s="27"/>
       <c r="C20" s="10">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F20" s="5"/>
       <c r="G20" s="4"/>
@@ -1479,17 +1490,17 @@
       <c r="J20" s="6"/>
     </row>
     <row r="21" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="21"/>
-      <c r="B21" s="24"/>
+      <c r="A21" s="20"/>
+      <c r="B21" s="27"/>
       <c r="C21" s="10">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F21" s="5"/>
       <c r="G21" s="4"/>
@@ -1498,17 +1509,17 @@
       <c r="J21" s="6"/>
     </row>
     <row r="22" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="21"/>
-      <c r="B22" s="24"/>
+      <c r="A22" s="20"/>
+      <c r="B22" s="27"/>
       <c r="C22" s="10">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F22" s="5"/>
       <c r="G22" s="4"/>
@@ -1517,51 +1528,69 @@
       <c r="J22" s="6"/>
     </row>
     <row r="23" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="21"/>
-      <c r="B23" s="25"/>
+      <c r="A23" s="20"/>
+      <c r="B23" s="27"/>
       <c r="C23" s="10">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="D23" s="16" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
       <c r="G23" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
       <c r="J23" s="6"/>
     </row>
     <row r="24" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="22"/>
-      <c r="B24" s="17" t="s">
+      <c r="A24" s="20"/>
+      <c r="B24" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="C24" s="10">
+      <c r="C24" s="36">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D24" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5" t="s">
+      <c r="E24" s="5" t="s">
         <v>11</v>
       </c>
+      <c r="F24" s="5"/>
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
       <c r="J24" s="6"/>
     </row>
+    <row r="25" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="21"/>
+      <c r="B25" s="38"/>
+      <c r="C25" s="36">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="D25" s="41" t="s">
+        <v>50</v>
+      </c>
+      <c r="E25" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="F25" s="5"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="6"/>
+    </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D28" s="19"/>
+      <c r="D28" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="A15:A24"/>
+  <mergeCells count="10">
     <mergeCell ref="B15:B23"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:B2"/>
@@ -1570,6 +1599,8 @@
     <mergeCell ref="A9:A14"/>
     <mergeCell ref="B9:B12"/>
     <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="A15:A25"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
[ATUALIZAÇÂO] - Art 15. 17.
</commit_message>
<xml_diff>
--- a/Documentation/17-Analise_dos_Eventos_para_cada_Cenario.xlsx
+++ b/Documentation/17-Analise_dos_Eventos_para_cada_Cenario.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/eed59d4ebf12600b/Documentos/Projeto/Faculdade/Silpan/Documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bc490d82787b51a2/Documentos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="84" documentId="11_F39CB75E9DCB1E95483200DF1B9D68301C93800A" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{EED2EF43-0E5A-4B72-BEAB-719CF1BB692C}"/>
+  <xr:revisionPtr revIDLastSave="230" documentId="8_{76FC5D5F-DBAD-408C-BCAE-F93491C61B30}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F53A1362-0910-4726-ACFD-AC7713B171C2}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="480" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DFD Orçamento sob medida" sheetId="5" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="71">
   <si>
     <t>Capacidades</t>
   </si>
@@ -183,9 +183,6 @@
     <t>Tratar pedido</t>
   </si>
   <si>
-    <t>Cliente efetua pagamento em dinheiro</t>
-  </si>
-  <si>
     <t>x(8)</t>
   </si>
   <si>
@@ -204,12 +201,6 @@
     <t>x(13)</t>
   </si>
   <si>
-    <t>x(16, 17)</t>
-  </si>
-  <si>
-    <t>x(18)</t>
-  </si>
-  <si>
     <t>x(19)</t>
   </si>
   <si>
@@ -219,9 +210,6 @@
     <t>x(20)</t>
   </si>
   <si>
-    <t>Cliente efetua pagamento cartão ou Pix</t>
-  </si>
-  <si>
     <t>x(22)</t>
   </si>
   <si>
@@ -234,14 +222,77 @@
     <t>x(14)</t>
   </si>
   <si>
-    <t>x(15, 23)</t>
+    <t>Tratar pagamento em dinheiro</t>
+  </si>
+  <si>
+    <t>Cliente informa número do pedido</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cliente não realiza o pagamento </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tratar pagamento com cartão </t>
+  </si>
+  <si>
+    <t>Cliente realiza pagamento em dinheiro</t>
+  </si>
+  <si>
+    <t>Cliente realiza pagamento com cartão</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tratar pagamento com Pix </t>
+  </si>
+  <si>
+    <t>Cliente realiza pagamento com Pix</t>
+  </si>
+  <si>
+    <t>Tratar empacotamento</t>
+  </si>
+  <si>
+    <t>Tratar devolução do pedido</t>
+  </si>
+  <si>
+    <t>Tratar troca do pedido</t>
+  </si>
+  <si>
+    <t>Cliente solicita devoluçao</t>
+  </si>
+  <si>
+    <t>Cliente solicita troca</t>
+  </si>
+  <si>
+    <t>Cliente entrega produto</t>
+  </si>
+  <si>
+    <t>Tratar estorno</t>
+  </si>
+  <si>
+    <t>Vendedor realiza troca</t>
+  </si>
+  <si>
+    <t>Cliente não entrega produto</t>
+  </si>
+  <si>
+    <t>Cliente entrega comprovante de pagamento</t>
+  </si>
+  <si>
+    <t>Caixa entrega comprovante de estorno</t>
+  </si>
+  <si>
+    <t>x(17)</t>
+  </si>
+  <si>
+    <t>x(15, 18)</t>
+  </si>
+  <si>
+    <t>x(25)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -288,20 +339,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -335,7 +372,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="34">
     <border>
       <left/>
       <right/>
@@ -555,21 +592,6 @@
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
       <top/>
       <bottom style="medium">
         <color rgb="FF000000"/>
@@ -629,15 +651,149 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top style="medium">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </top>
       <bottom style="medium">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -645,7 +801,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -680,32 +836,31 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -716,53 +871,139 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1078,37 +1319,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:J46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
     <col min="4" max="4" width="52.28515625" customWidth="1"/>
     <col min="5" max="5" width="12.5703125" customWidth="1"/>
     <col min="6" max="6" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="22"/>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
+      <c r="A1" s="21"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
     </row>
     <row r="2" spans="1:10" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="25"/>
+      <c r="B2" s="24"/>
       <c r="C2" s="8" t="s">
         <v>1</v>
       </c>
@@ -1135,10 +1376,10 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="16.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="19" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="9">
@@ -1157,8 +1398,8 @@
       <c r="J3" s="6"/>
     </row>
     <row r="4" spans="1:10" ht="16.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="20"/>
-      <c r="B4" s="27"/>
+      <c r="A4" s="27"/>
+      <c r="B4" s="20"/>
       <c r="C4" s="10">
         <f>C3+1</f>
         <v>2</v>
@@ -1176,10 +1417,10 @@
       <c r="J4" s="6"/>
     </row>
     <row r="5" spans="1:10" ht="16.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="20"/>
-      <c r="B5" s="27"/>
+      <c r="A5" s="27"/>
+      <c r="B5" s="20"/>
       <c r="C5" s="10">
-        <f t="shared" ref="C5:C25" si="0">C4+1</f>
+        <f t="shared" ref="C5:C41" si="0">C4+1</f>
         <v>3</v>
       </c>
       <c r="D5" s="7" t="s">
@@ -1195,8 +1436,8 @@
       <c r="J5" s="6"/>
     </row>
     <row r="6" spans="1:10" ht="16.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="20"/>
-      <c r="B6" s="27"/>
+      <c r="A6" s="27"/>
+      <c r="B6" s="20"/>
       <c r="C6" s="10">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1214,8 +1455,8 @@
       <c r="J6" s="6"/>
     </row>
     <row r="7" spans="1:10" ht="16.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="20"/>
-      <c r="B7" s="27"/>
+      <c r="A7" s="27"/>
+      <c r="B7" s="20"/>
       <c r="C7" s="10">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1233,8 +1474,8 @@
       <c r="J7" s="6"/>
     </row>
     <row r="8" spans="1:10" ht="16.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="21"/>
-      <c r="B8" s="28"/>
+      <c r="A8" s="28"/>
+      <c r="B8" s="25"/>
       <c r="C8" s="10">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1306,7 +1547,7 @@
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
       <c r="G11" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
@@ -1325,7 +1566,7 @@
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
       <c r="G12" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
@@ -1348,55 +1589,55 @@
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
       <c r="I13" s="15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J13" s="14"/>
     </row>
     <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="31"/>
-      <c r="B14" s="35"/>
-      <c r="C14" s="10">
+      <c r="B14" s="42"/>
+      <c r="C14" s="43">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="39" t="s">
+        <v>39</v>
+      </c>
+      <c r="F14" s="39"/>
+      <c r="G14" s="40"/>
+      <c r="H14" s="40"/>
+      <c r="I14" s="40"/>
+      <c r="J14" s="41"/>
+    </row>
+    <row r="15" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="9">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="D15" s="45" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="46" t="s">
         <v>40</v>
       </c>
-      <c r="F14" s="5"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="6"/>
-    </row>
-    <row r="15" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="B15" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" s="10">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="F15" s="5"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="6"/>
+      <c r="F15" s="46"/>
+      <c r="G15" s="47"/>
+      <c r="H15" s="47"/>
+      <c r="I15" s="47"/>
+      <c r="J15" s="48"/>
     </row>
     <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="20"/>
-      <c r="B16" s="27"/>
+      <c r="A16" s="27"/>
+      <c r="B16" s="20"/>
       <c r="C16" s="10">
         <f>C15+1</f>
         <v>14</v>
@@ -1407,191 +1648,527 @@
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
       <c r="G16" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
-      <c r="J16" s="6"/>
+      <c r="J16" s="49"/>
     </row>
     <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="20"/>
-      <c r="B17" s="27"/>
+      <c r="A17" s="27"/>
+      <c r="B17" s="20"/>
       <c r="C17" s="10">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
-      <c r="J17" s="6"/>
+      <c r="J17" s="49"/>
     </row>
     <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="20"/>
-      <c r="B18" s="27"/>
-      <c r="C18" s="10">
+      <c r="A18" s="27"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="9">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="D18" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>53</v>
-      </c>
+      <c r="D18" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" s="5"/>
       <c r="F18" s="5"/>
-      <c r="G18" s="4"/>
+      <c r="G18" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
-      <c r="J18" s="6"/>
+      <c r="J18" s="49"/>
     </row>
     <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="20"/>
-      <c r="B19" s="27"/>
+      <c r="A19" s="27"/>
+      <c r="B19" s="35" t="s">
+        <v>25</v>
+      </c>
       <c r="C19" s="10">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="D19" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F19" s="5"/>
+      <c r="D19" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5" t="s">
+        <v>11</v>
+      </c>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
-      <c r="J19" s="6"/>
+      <c r="J19" s="49"/>
     </row>
     <row r="20" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="20"/>
-      <c r="B20" s="27"/>
+      <c r="A20" s="27"/>
+      <c r="B20" s="36"/>
       <c r="C20" s="10">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D20" s="37" t="s">
+        <v>46</v>
+      </c>
+      <c r="E20" s="38"/>
+      <c r="F20" s="39"/>
+      <c r="G20" s="40" t="s">
+        <v>68</v>
+      </c>
+      <c r="H20" s="40"/>
+      <c r="I20" s="40"/>
+      <c r="J20" s="50"/>
+    </row>
+    <row r="21" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" s="60" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="9">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="D21" s="62" t="s">
+        <v>50</v>
+      </c>
+      <c r="E21" s="65" t="s">
+        <v>69</v>
+      </c>
+      <c r="F21" s="56"/>
+      <c r="G21" s="54"/>
+      <c r="H21" s="54"/>
+      <c r="I21" s="53"/>
+      <c r="J21" s="52"/>
+    </row>
+    <row r="22" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="27"/>
+      <c r="B22" s="61"/>
+      <c r="C22" s="10">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="D22" s="63" t="s">
+        <v>53</v>
+      </c>
+      <c r="E22" s="66" t="s">
+        <v>42</v>
+      </c>
+      <c r="F22" s="57"/>
+      <c r="G22" s="55"/>
+      <c r="H22" s="55"/>
+      <c r="I22" s="54"/>
+      <c r="J22" s="58"/>
+    </row>
+    <row r="23" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="27"/>
+      <c r="B23" s="59" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="10">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="D23" s="64" t="s">
+        <v>51</v>
+      </c>
+      <c r="E23" s="66"/>
+      <c r="F23" s="70" t="s">
+        <v>69</v>
+      </c>
+      <c r="G23" s="55"/>
+      <c r="H23" s="55"/>
+      <c r="I23" s="55"/>
+      <c r="J23" s="58"/>
+    </row>
+    <row r="24" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" s="60" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="9">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="D24" s="62" t="s">
+        <v>50</v>
+      </c>
+      <c r="E24" s="65" t="s">
+        <v>69</v>
+      </c>
+      <c r="F24" s="56"/>
+      <c r="G24" s="54"/>
+      <c r="H24" s="54"/>
+      <c r="I24" s="53"/>
+      <c r="J24" s="52"/>
+    </row>
+    <row r="25" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="27"/>
+      <c r="B25" s="61"/>
+      <c r="C25" s="10">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="D25" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="E25" s="66" t="s">
+        <v>45</v>
+      </c>
+      <c r="F25" s="57"/>
+      <c r="G25" s="55"/>
+      <c r="H25" s="55"/>
+      <c r="I25" s="54"/>
+      <c r="J25" s="58"/>
+    </row>
+    <row r="26" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="27"/>
+      <c r="B26" s="59" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" s="10">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="D26" s="64" t="s">
+        <v>51</v>
+      </c>
+      <c r="E26" s="66"/>
+      <c r="F26" s="70" t="s">
+        <v>69</v>
+      </c>
+      <c r="G26" s="55"/>
+      <c r="H26" s="55"/>
+      <c r="I26" s="55"/>
+      <c r="J26" s="58"/>
+    </row>
+    <row r="27" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="B27" s="60" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" s="9">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="D27" s="62" t="s">
+        <v>50</v>
+      </c>
+      <c r="E27" s="65" t="s">
+        <v>69</v>
+      </c>
+      <c r="F27" s="56"/>
+      <c r="G27" s="54"/>
+      <c r="H27" s="54"/>
+      <c r="I27" s="53"/>
+      <c r="J27" s="52"/>
+    </row>
+    <row r="28" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="27"/>
+      <c r="B28" s="61"/>
+      <c r="C28" s="9">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="D28" s="63" t="s">
+        <v>56</v>
+      </c>
+      <c r="E28" s="66" t="s">
+        <v>70</v>
+      </c>
+      <c r="F28" s="57"/>
+      <c r="G28" s="55"/>
+      <c r="H28" s="55"/>
+      <c r="I28" s="54"/>
+      <c r="J28" s="58"/>
+    </row>
+    <row r="29" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="27"/>
+      <c r="B29" s="59" t="s">
+        <v>25</v>
+      </c>
+      <c r="C29" s="9">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="D29" s="64" t="s">
+        <v>51</v>
+      </c>
+      <c r="E29" s="66"/>
+      <c r="F29" s="70" t="s">
+        <v>69</v>
+      </c>
+      <c r="G29" s="55"/>
+      <c r="H29" s="55"/>
+      <c r="I29" s="55"/>
+      <c r="J29" s="58"/>
+    </row>
+    <row r="30" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="B30" s="60" t="s">
+        <v>9</v>
+      </c>
+      <c r="C30" s="9">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="D30" s="62" t="s">
         <v>29</v>
       </c>
-      <c r="E20" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="F20" s="5"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="6"/>
-    </row>
-    <row r="21" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="20"/>
-      <c r="B21" s="27"/>
-      <c r="C21" s="10">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="D21" s="3" t="s">
+      <c r="E30" s="65"/>
+      <c r="F30" s="56"/>
+      <c r="G30" s="54" t="s">
+        <v>11</v>
+      </c>
+      <c r="H30" s="54"/>
+      <c r="I30" s="53"/>
+      <c r="J30" s="52"/>
+    </row>
+    <row r="31" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="27"/>
+      <c r="B31" s="67"/>
+      <c r="C31" s="9">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="D31" s="63" t="s">
         <v>30</v>
       </c>
-      <c r="E21" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F21" s="5"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="6"/>
-    </row>
-    <row r="22" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="20"/>
-      <c r="B22" s="27"/>
-      <c r="C22" s="10">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="D22" s="3" t="s">
+      <c r="E31" s="66"/>
+      <c r="F31" s="57"/>
+      <c r="G31" s="55"/>
+      <c r="H31" s="55"/>
+      <c r="I31" s="53"/>
+      <c r="J31" s="52"/>
+    </row>
+    <row r="32" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="27"/>
+      <c r="B32" s="61"/>
+      <c r="C32" s="9">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="D32" s="63" t="s">
         <v>31</v>
       </c>
-      <c r="E22" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="F22" s="5"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="6"/>
-    </row>
-    <row r="23" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="20"/>
-      <c r="B23" s="27"/>
-      <c r="C23" s="10">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="D23" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="H23" s="4"/>
-      <c r="I23" s="4"/>
-      <c r="J23" s="6"/>
-    </row>
-    <row r="24" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="20"/>
-      <c r="B24" s="37" t="s">
+      <c r="E32" s="66"/>
+      <c r="F32" s="57"/>
+      <c r="G32" s="55"/>
+      <c r="H32" s="55"/>
+      <c r="I32" s="54"/>
+      <c r="J32" s="58"/>
+    </row>
+    <row r="33" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="B33" s="60" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" s="9">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="D33" s="62" t="s">
+        <v>60</v>
+      </c>
+      <c r="E33" s="65"/>
+      <c r="F33" s="56"/>
+      <c r="G33" s="54"/>
+      <c r="H33" s="54"/>
+      <c r="I33" s="53"/>
+      <c r="J33" s="52"/>
+    </row>
+    <row r="34" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="27"/>
+      <c r="B34" s="67"/>
+      <c r="C34" s="9">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="D34" s="63" t="s">
+        <v>62</v>
+      </c>
+      <c r="E34" s="66"/>
+      <c r="F34" s="57"/>
+      <c r="G34" s="55"/>
+      <c r="H34" s="55"/>
+      <c r="I34" s="53"/>
+      <c r="J34" s="52"/>
+    </row>
+    <row r="35" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="17"/>
+      <c r="B35" s="59" t="s">
         <v>25</v>
       </c>
-      <c r="C24" s="36">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="D24" s="40" t="s">
-        <v>22</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F24" s="5"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="4"/>
-      <c r="J24" s="6"/>
-    </row>
-    <row r="25" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="21"/>
-      <c r="B25" s="38"/>
-      <c r="C25" s="36">
-        <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-      <c r="D25" s="41" t="s">
-        <v>50</v>
-      </c>
-      <c r="E25" s="39" t="s">
-        <v>49</v>
-      </c>
-      <c r="F25" s="5"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="4"/>
-      <c r="J25" s="6"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D28" s="18"/>
+      <c r="C35" s="9">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="D35" s="63" t="s">
+        <v>65</v>
+      </c>
+      <c r="E35" s="66"/>
+      <c r="F35" s="57"/>
+      <c r="G35" s="55"/>
+      <c r="H35" s="55"/>
+      <c r="I35" s="53"/>
+      <c r="J35" s="52"/>
+    </row>
+    <row r="36" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="B36" s="60" t="s">
+        <v>9</v>
+      </c>
+      <c r="C36" s="9">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="D36" s="63" t="s">
+        <v>61</v>
+      </c>
+      <c r="E36" s="66"/>
+      <c r="F36" s="57"/>
+      <c r="G36" s="55"/>
+      <c r="H36" s="55"/>
+      <c r="I36" s="54"/>
+      <c r="J36" s="58"/>
+    </row>
+    <row r="37" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="27"/>
+      <c r="B37" s="67"/>
+      <c r="C37" s="9">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="D37" s="63" t="s">
+        <v>62</v>
+      </c>
+      <c r="E37" s="66"/>
+      <c r="F37" s="57"/>
+      <c r="G37" s="55"/>
+      <c r="H37" s="55"/>
+      <c r="I37" s="53"/>
+      <c r="J37" s="52"/>
+    </row>
+    <row r="38" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="27"/>
+      <c r="B38" s="61"/>
+      <c r="C38" s="9">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="D38" s="63" t="s">
+        <v>64</v>
+      </c>
+      <c r="E38" s="66"/>
+      <c r="F38" s="57"/>
+      <c r="G38" s="55"/>
+      <c r="H38" s="55"/>
+      <c r="I38" s="54"/>
+      <c r="J38" s="58"/>
+    </row>
+    <row r="39" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="17"/>
+      <c r="B39" s="68" t="s">
+        <v>25</v>
+      </c>
+      <c r="C39" s="9">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="D39" s="63" t="s">
+        <v>65</v>
+      </c>
+      <c r="E39" s="66"/>
+      <c r="F39" s="57"/>
+      <c r="G39" s="55"/>
+      <c r="H39" s="55"/>
+      <c r="I39" s="55"/>
+      <c r="J39" s="58"/>
+    </row>
+    <row r="40" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="B40" s="60" t="s">
+        <v>9</v>
+      </c>
+      <c r="C40" s="9">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="D40" s="62" t="s">
+        <v>66</v>
+      </c>
+      <c r="E40" s="65"/>
+      <c r="F40" s="56"/>
+      <c r="G40" s="54"/>
+      <c r="H40" s="54"/>
+      <c r="I40" s="53"/>
+      <c r="J40" s="52"/>
+    </row>
+    <row r="41" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="28"/>
+      <c r="B41" s="69"/>
+      <c r="C41" s="9">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="D41" s="63" t="s">
+        <v>67</v>
+      </c>
+      <c r="E41" s="66"/>
+      <c r="F41" s="57"/>
+      <c r="G41" s="55"/>
+      <c r="H41" s="55"/>
+      <c r="I41" s="53"/>
+      <c r="J41" s="52"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E46" s="51"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="B15:B23"/>
+  <mergeCells count="24">
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="A36:A38"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="A15:A20"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="B30:B32"/>
+    <mergeCell ref="B15:B18"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="B3:B8"/>
@@ -1599,8 +2176,6 @@
     <mergeCell ref="A9:A14"/>
     <mergeCell ref="B9:B12"/>
     <mergeCell ref="B13:B14"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="A15:A25"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
[ATUALIZAÇÃO] - Art 15.
</commit_message>
<xml_diff>
--- a/Documentation/17-Analise_dos_Eventos_para_cada_Cenario.xlsx
+++ b/Documentation/17-Analise_dos_Eventos_para_cada_Cenario.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bc490d82787b51a2/Documentos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/eed59d4ebf12600b/Documentos/Projeto/Faculdade/Silpan/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="230" documentId="8_{76FC5D5F-DBAD-408C-BCAE-F93491C61B30}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F53A1362-0910-4726-ACFD-AC7713B171C2}"/>
+  <xr:revisionPtr revIDLastSave="306" documentId="8_{76FC5D5F-DBAD-408C-BCAE-F93491C61B30}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{DB71B1B2-66BF-43FA-B25E-161F7C840BC8}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="480" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DFD Orçamento sob medida" sheetId="5" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="82">
   <si>
     <t>Capacidades</t>
   </si>
@@ -287,12 +287,45 @@
   <si>
     <t>x(25)</t>
   </si>
+  <si>
+    <t>Tratar compra de produtos</t>
+  </si>
+  <si>
+    <t>Abastecer estoque</t>
+  </si>
+  <si>
+    <t>Externo</t>
+  </si>
+  <si>
+    <t>Temporal</t>
+  </si>
+  <si>
+    <t>Assistente de Compras solicita orçamento</t>
+  </si>
+  <si>
+    <t>Assistente de Compras realiza compra</t>
+  </si>
+  <si>
+    <t>Fabricante entrega produtos</t>
+  </si>
+  <si>
+    <t>almoxarife atualiza produtos</t>
+  </si>
+  <si>
+    <t>Fabricante entrega orçamento</t>
+  </si>
+  <si>
+    <t>Consultor de compras analisa orçamento</t>
+  </si>
+  <si>
+    <t>Fabricantte não entrega produtos</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -339,6 +372,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -372,7 +411,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="34">
+  <borders count="39">
     <border>
       <left/>
       <right/>
@@ -797,11 +836,64 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -851,20 +943,128 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -874,15 +1074,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -901,109 +1092,47 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1319,10 +1448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J46"/>
+  <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34:A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1333,849 +1462,1028 @@
     <col min="6" max="6" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="21"/>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-    </row>
-    <row r="2" spans="1:10" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="23" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="70"/>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="78" t="s">
+        <v>73</v>
+      </c>
+      <c r="F1" s="79"/>
+      <c r="G1" s="72" t="s">
+        <v>74</v>
+      </c>
+      <c r="H1" s="76"/>
+      <c r="I1" s="73"/>
+    </row>
+    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="69"/>
+      <c r="B2" s="69"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="75"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="77"/>
+      <c r="I2" s="75"/>
+      <c r="J2" s="18"/>
+    </row>
+    <row r="3" spans="1:10" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="8" t="s">
+      <c r="B3" s="60"/>
+      <c r="C3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E3" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F3" s="71" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G3" s="71" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H3" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I3" s="71" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="16.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="26" t="s">
+    <row r="4" spans="1:10" ht="16.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B4" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C4" s="9">
         <v>1</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5" t="s">
+      <c r="E4" s="5"/>
+      <c r="F4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="6"/>
-    </row>
-    <row r="4" spans="1:10" ht="16.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="27"/>
-      <c r="B4" s="20"/>
-      <c r="C4" s="10">
-        <f>C3+1</f>
-        <v>2</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="4" t="s">
-        <v>13</v>
-      </c>
+      <c r="G4" s="4"/>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
       <c r="J4" s="6"/>
     </row>
     <row r="5" spans="1:10" ht="16.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="27"/>
-      <c r="B5" s="20"/>
+      <c r="A5" s="49"/>
+      <c r="B5" s="58"/>
       <c r="C5" s="10">
-        <f t="shared" ref="C5:C41" si="0">C4+1</f>
-        <v>3</v>
+        <f>C4+1</f>
+        <v>2</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>15</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="E5" s="5"/>
       <c r="F5" s="5"/>
-      <c r="G5" s="4"/>
+      <c r="G5" s="4" t="s">
+        <v>13</v>
+      </c>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
       <c r="J5" s="6"/>
     </row>
     <row r="6" spans="1:10" ht="16.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="27"/>
-      <c r="B6" s="20"/>
+      <c r="A6" s="49"/>
+      <c r="B6" s="58"/>
       <c r="C6" s="10">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <f t="shared" ref="C6:C51" si="0">C5+1</f>
+        <v>3</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="5"/>
+        <v>14</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="F6" s="5"/>
-      <c r="G6" s="4" t="s">
-        <v>17</v>
-      </c>
+      <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
       <c r="J6" s="6"/>
     </row>
     <row r="7" spans="1:10" ht="16.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="27"/>
-      <c r="B7" s="20"/>
+      <c r="A7" s="49"/>
+      <c r="B7" s="58"/>
       <c r="C7" s="10">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>19</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="E7" s="5"/>
       <c r="F7" s="5"/>
-      <c r="G7" s="4"/>
+      <c r="G7" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
       <c r="J7" s="6"/>
     </row>
     <row r="8" spans="1:10" ht="16.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="28"/>
-      <c r="B8" s="25"/>
+      <c r="A8" s="49"/>
+      <c r="B8" s="58"/>
       <c r="C8" s="10">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="5"/>
+        <v>18</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="F8" s="5"/>
-      <c r="G8" s="4" t="s">
-        <v>21</v>
-      </c>
+      <c r="G8" s="4"/>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
       <c r="J8" s="6"/>
     </row>
-    <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="29" t="s">
+    <row r="9" spans="1:10" ht="16.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="53"/>
+      <c r="B9" s="61"/>
+      <c r="C9" s="10">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="6"/>
+    </row>
+    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="62" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="32" t="s">
+      <c r="B10" s="65" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C10" s="10">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D10" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12" t="s">
+      <c r="E10" s="12"/>
+      <c r="F10" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="14"/>
-    </row>
-    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="30"/>
-      <c r="B10" s="33"/>
-      <c r="C10" s="10">
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="14"/>
+    </row>
+    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="63"/>
+      <c r="B11" s="66"/>
+      <c r="C11" s="10">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D11" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E11" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F10" s="5"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="6"/>
-    </row>
-    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="30"/>
-      <c r="B11" s="33"/>
-      <c r="C11" s="10">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E11" s="5"/>
       <c r="F11" s="5"/>
-      <c r="G11" s="4" t="s">
-        <v>36</v>
-      </c>
+      <c r="G11" s="4"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
       <c r="J11" s="6"/>
     </row>
     <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="30"/>
-      <c r="B12" s="33"/>
+      <c r="A12" s="63"/>
+      <c r="B12" s="66"/>
       <c r="C12" s="10">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
       <c r="G12" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
       <c r="J12" s="6"/>
     </row>
     <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="31"/>
-      <c r="B13" s="34" t="s">
+      <c r="A13" s="63"/>
+      <c r="B13" s="66"/>
+      <c r="C13" s="10">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="6"/>
+    </row>
+    <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="64"/>
+      <c r="B14" s="67" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C14" s="10">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D14" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="15" t="s">
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="J13" s="14"/>
-    </row>
-    <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="31"/>
-      <c r="B14" s="42"/>
-      <c r="C14" s="43">
+      <c r="J14" s="14"/>
+    </row>
+    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="64"/>
+      <c r="B15" s="68"/>
+      <c r="C15" s="24">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="D14" s="44" t="s">
+      <c r="D15" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="E14" s="39" t="s">
+      <c r="E15" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="F14" s="39"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="40"/>
-      <c r="I14" s="40"/>
-      <c r="J14" s="41"/>
-    </row>
-    <row r="15" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="26" t="s">
+      <c r="F15" s="21"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="22"/>
+      <c r="J15" s="23"/>
+    </row>
+    <row r="16" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="19" t="s">
+      <c r="B16" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="9">
+      <c r="C16" s="9">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="D15" s="45" t="s">
+      <c r="D16" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="E15" s="46" t="s">
+      <c r="E16" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="F15" s="46"/>
-      <c r="G15" s="47"/>
-      <c r="H15" s="47"/>
-      <c r="I15" s="47"/>
-      <c r="J15" s="48"/>
-    </row>
-    <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="27"/>
-      <c r="B16" s="20"/>
-      <c r="C16" s="10">
-        <f>C15+1</f>
+      <c r="F16" s="27"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="28"/>
+      <c r="I16" s="28"/>
+      <c r="J16" s="29"/>
+    </row>
+    <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="49"/>
+      <c r="B17" s="58"/>
+      <c r="C17" s="10">
+        <f>C16+1</f>
         <v>14</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D17" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="49"/>
-    </row>
-    <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="27"/>
-      <c r="B17" s="20"/>
-      <c r="C17" s="10">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>47</v>
       </c>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="4" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
-      <c r="J17" s="49"/>
+      <c r="J17" s="30"/>
     </row>
     <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="27"/>
-      <c r="B18" s="20"/>
-      <c r="C18" s="9">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="D18" s="16" t="s">
-        <v>43</v>
+      <c r="A18" s="49"/>
+      <c r="B18" s="58"/>
+      <c r="C18" s="10">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
       <c r="G18" s="4" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
-      <c r="J18" s="49"/>
+      <c r="J18" s="30"/>
     </row>
     <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="27"/>
-      <c r="B19" s="35" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19" s="10">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="D19" s="18" t="s">
-        <v>22</v>
+      <c r="A19" s="49"/>
+      <c r="B19" s="58"/>
+      <c r="C19" s="9">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>43</v>
       </c>
       <c r="E19" s="5"/>
-      <c r="F19" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G19" s="4"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
-      <c r="J19" s="49"/>
+      <c r="J19" s="30"/>
     </row>
     <row r="20" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="27"/>
-      <c r="B20" s="36"/>
+      <c r="A20" s="49"/>
+      <c r="B20" s="55" t="s">
+        <v>25</v>
+      </c>
       <c r="C20" s="10">
         <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="30"/>
+    </row>
+    <row r="21" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="49"/>
+      <c r="B21" s="56"/>
+      <c r="C21" s="10">
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="D20" s="37" t="s">
+      <c r="D21" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="E20" s="38"/>
-      <c r="F20" s="39"/>
-      <c r="G20" s="40" t="s">
+      <c r="E21" s="20"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="H20" s="40"/>
-      <c r="I20" s="40"/>
-      <c r="J20" s="50"/>
-    </row>
-    <row r="21" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="26" t="s">
+      <c r="H21" s="22"/>
+      <c r="I21" s="22"/>
+      <c r="J21" s="31"/>
+    </row>
+    <row r="22" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="B21" s="60" t="s">
+      <c r="B22" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="C21" s="9">
+      <c r="C22" s="9">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="D21" s="62" t="s">
+      <c r="D22" s="40" t="s">
         <v>50</v>
       </c>
-      <c r="E21" s="65" t="s">
+      <c r="E22" s="43" t="s">
         <v>69</v>
       </c>
-      <c r="F21" s="56"/>
-      <c r="G21" s="54"/>
-      <c r="H21" s="54"/>
-      <c r="I21" s="53"/>
-      <c r="J21" s="52"/>
-    </row>
-    <row r="22" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="27"/>
-      <c r="B22" s="61"/>
-      <c r="C22" s="10">
+      <c r="F22" s="36"/>
+      <c r="G22" s="34"/>
+      <c r="H22" s="34"/>
+      <c r="I22" s="33"/>
+      <c r="J22" s="32"/>
+    </row>
+    <row r="23" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="49"/>
+      <c r="B23" s="52"/>
+      <c r="C23" s="10">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="D22" s="63" t="s">
+      <c r="D23" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="E22" s="66" t="s">
+      <c r="E23" s="44" t="s">
         <v>42</v>
       </c>
-      <c r="F22" s="57"/>
-      <c r="G22" s="55"/>
-      <c r="H22" s="55"/>
-      <c r="I22" s="54"/>
-      <c r="J22" s="58"/>
-    </row>
-    <row r="23" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="27"/>
-      <c r="B23" s="59" t="s">
+      <c r="F23" s="37"/>
+      <c r="G23" s="35"/>
+      <c r="H23" s="35"/>
+      <c r="I23" s="34"/>
+      <c r="J23" s="38"/>
+    </row>
+    <row r="24" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="49"/>
+      <c r="B24" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="10">
+      <c r="C24" s="10">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="D23" s="64" t="s">
+      <c r="D24" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="E23" s="66"/>
-      <c r="F23" s="70" t="s">
+      <c r="E24" s="44"/>
+      <c r="F24" s="47" t="s">
         <v>69</v>
       </c>
-      <c r="G23" s="55"/>
-      <c r="H23" s="55"/>
-      <c r="I23" s="55"/>
-      <c r="J23" s="58"/>
-    </row>
-    <row r="24" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="26" t="s">
+      <c r="G24" s="35"/>
+      <c r="H24" s="35"/>
+      <c r="I24" s="35"/>
+      <c r="J24" s="38"/>
+    </row>
+    <row r="25" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="48" t="s">
         <v>52</v>
       </c>
-      <c r="B24" s="60" t="s">
+      <c r="B25" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="9">
+      <c r="C25" s="9">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="D24" s="62" t="s">
+      <c r="D25" s="40" t="s">
         <v>50</v>
       </c>
-      <c r="E24" s="65" t="s">
+      <c r="E25" s="43" t="s">
         <v>69</v>
       </c>
-      <c r="F24" s="56"/>
-      <c r="G24" s="54"/>
-      <c r="H24" s="54"/>
-      <c r="I24" s="53"/>
-      <c r="J24" s="52"/>
-    </row>
-    <row r="25" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="27"/>
-      <c r="B25" s="61"/>
-      <c r="C25" s="10">
+      <c r="F25" s="36"/>
+      <c r="G25" s="34"/>
+      <c r="H25" s="34"/>
+      <c r="I25" s="33"/>
+      <c r="J25" s="32"/>
+    </row>
+    <row r="26" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="49"/>
+      <c r="B26" s="52"/>
+      <c r="C26" s="10">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="D25" s="63" t="s">
+      <c r="D26" s="41" t="s">
         <v>54</v>
       </c>
-      <c r="E25" s="66" t="s">
+      <c r="E26" s="44" t="s">
         <v>45</v>
       </c>
-      <c r="F25" s="57"/>
-      <c r="G25" s="55"/>
-      <c r="H25" s="55"/>
-      <c r="I25" s="54"/>
-      <c r="J25" s="58"/>
-    </row>
-    <row r="26" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="27"/>
-      <c r="B26" s="59" t="s">
+      <c r="F26" s="37"/>
+      <c r="G26" s="35"/>
+      <c r="H26" s="35"/>
+      <c r="I26" s="34"/>
+      <c r="J26" s="38"/>
+    </row>
+    <row r="27" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="49"/>
+      <c r="B27" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="C26" s="10">
+      <c r="C27" s="10">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="D26" s="64" t="s">
+      <c r="D27" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="E26" s="66"/>
-      <c r="F26" s="70" t="s">
+      <c r="E27" s="44"/>
+      <c r="F27" s="47" t="s">
         <v>69</v>
       </c>
-      <c r="G26" s="55"/>
-      <c r="H26" s="55"/>
-      <c r="I26" s="55"/>
-      <c r="J26" s="58"/>
-    </row>
-    <row r="27" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="26" t="s">
+      <c r="G27" s="35"/>
+      <c r="H27" s="35"/>
+      <c r="I27" s="35"/>
+      <c r="J27" s="38"/>
+    </row>
+    <row r="28" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="48" t="s">
         <v>55</v>
       </c>
-      <c r="B27" s="60" t="s">
+      <c r="B28" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="C27" s="9">
+      <c r="C28" s="9">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="D27" s="62" t="s">
+      <c r="D28" s="40" t="s">
         <v>50</v>
       </c>
-      <c r="E27" s="65" t="s">
+      <c r="E28" s="43" t="s">
         <v>69</v>
       </c>
-      <c r="F27" s="56"/>
-      <c r="G27" s="54"/>
-      <c r="H27" s="54"/>
-      <c r="I27" s="53"/>
-      <c r="J27" s="52"/>
-    </row>
-    <row r="28" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="27"/>
-      <c r="B28" s="61"/>
-      <c r="C28" s="9">
+      <c r="F28" s="36"/>
+      <c r="G28" s="34"/>
+      <c r="H28" s="34"/>
+      <c r="I28" s="33"/>
+      <c r="J28" s="32"/>
+    </row>
+    <row r="29" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="49"/>
+      <c r="B29" s="52"/>
+      <c r="C29" s="9">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="D28" s="63" t="s">
+      <c r="D29" s="41" t="s">
         <v>56</v>
       </c>
-      <c r="E28" s="66" t="s">
+      <c r="E29" s="44" t="s">
         <v>70</v>
       </c>
-      <c r="F28" s="57"/>
-      <c r="G28" s="55"/>
-      <c r="H28" s="55"/>
-      <c r="I28" s="54"/>
-      <c r="J28" s="58"/>
-    </row>
-    <row r="29" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="27"/>
-      <c r="B29" s="59" t="s">
+      <c r="F29" s="37"/>
+      <c r="G29" s="35"/>
+      <c r="H29" s="35"/>
+      <c r="I29" s="34"/>
+      <c r="J29" s="38"/>
+    </row>
+    <row r="30" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="49"/>
+      <c r="B30" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="C29" s="9">
+      <c r="C30" s="9">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="D29" s="64" t="s">
+      <c r="D30" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="E29" s="66"/>
-      <c r="F29" s="70" t="s">
+      <c r="E30" s="44"/>
+      <c r="F30" s="47" t="s">
         <v>69</v>
       </c>
-      <c r="G29" s="55"/>
-      <c r="H29" s="55"/>
-      <c r="I29" s="55"/>
-      <c r="J29" s="58"/>
-    </row>
-    <row r="30" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="26" t="s">
+      <c r="G30" s="35"/>
+      <c r="H30" s="35"/>
+      <c r="I30" s="35"/>
+      <c r="J30" s="38"/>
+    </row>
+    <row r="31" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="48" t="s">
         <v>57</v>
       </c>
-      <c r="B30" s="60" t="s">
+      <c r="B31" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="C30" s="9">
+      <c r="C31" s="9">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="D30" s="62" t="s">
+      <c r="D31" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="E30" s="65"/>
-      <c r="F30" s="56"/>
-      <c r="G30" s="54" t="s">
+      <c r="E31" s="43"/>
+      <c r="F31" s="36"/>
+      <c r="G31" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="H30" s="54"/>
-      <c r="I30" s="53"/>
-      <c r="J30" s="52"/>
-    </row>
-    <row r="31" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="27"/>
-      <c r="B31" s="67"/>
-      <c r="C31" s="9">
+      <c r="H31" s="34"/>
+      <c r="I31" s="33"/>
+      <c r="J31" s="32"/>
+    </row>
+    <row r="32" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="49"/>
+      <c r="B32" s="51"/>
+      <c r="C32" s="9">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="D31" s="63" t="s">
+      <c r="D32" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="E31" s="66"/>
-      <c r="F31" s="57"/>
-      <c r="G31" s="55"/>
-      <c r="H31" s="55"/>
-      <c r="I31" s="53"/>
-      <c r="J31" s="52"/>
-    </row>
-    <row r="32" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="27"/>
-      <c r="B32" s="61"/>
-      <c r="C32" s="9">
+      <c r="E32" s="44"/>
+      <c r="F32" s="37"/>
+      <c r="G32" s="35"/>
+      <c r="H32" s="35"/>
+      <c r="I32" s="33"/>
+      <c r="J32" s="32"/>
+    </row>
+    <row r="33" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="49"/>
+      <c r="B33" s="52"/>
+      <c r="C33" s="9">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="D32" s="63" t="s">
+      <c r="D33" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="E32" s="66"/>
-      <c r="F32" s="57"/>
-      <c r="G32" s="55"/>
-      <c r="H32" s="55"/>
-      <c r="I32" s="54"/>
-      <c r="J32" s="58"/>
-    </row>
-    <row r="33" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="26" t="s">
+      <c r="E33" s="44"/>
+      <c r="F33" s="37"/>
+      <c r="G33" s="35"/>
+      <c r="H33" s="35"/>
+      <c r="I33" s="34"/>
+      <c r="J33" s="38"/>
+    </row>
+    <row r="34" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="48" t="s">
         <v>58</v>
       </c>
-      <c r="B33" s="60" t="s">
+      <c r="B34" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="C33" s="9">
+      <c r="C34" s="9">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="D33" s="62" t="s">
+      <c r="D34" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="E33" s="65"/>
-      <c r="F33" s="56"/>
-      <c r="G33" s="54"/>
-      <c r="H33" s="54"/>
-      <c r="I33" s="53"/>
-      <c r="J33" s="52"/>
-    </row>
-    <row r="34" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="27"/>
-      <c r="B34" s="67"/>
-      <c r="C34" s="9">
+      <c r="E34" s="43"/>
+      <c r="F34" s="36"/>
+      <c r="G34" s="34"/>
+      <c r="H34" s="34"/>
+      <c r="I34" s="33"/>
+      <c r="J34" s="32"/>
+    </row>
+    <row r="35" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="49"/>
+      <c r="B35" s="51"/>
+      <c r="C35" s="9">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="D34" s="63" t="s">
+      <c r="D35" s="41" t="s">
         <v>62</v>
       </c>
-      <c r="E34" s="66"/>
-      <c r="F34" s="57"/>
-      <c r="G34" s="55"/>
-      <c r="H34" s="55"/>
-      <c r="I34" s="53"/>
-      <c r="J34" s="52"/>
-    </row>
-    <row r="35" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="17"/>
-      <c r="B35" s="59" t="s">
+      <c r="E35" s="44"/>
+      <c r="F35" s="37"/>
+      <c r="G35" s="35"/>
+      <c r="H35" s="35"/>
+      <c r="I35" s="33"/>
+      <c r="J35" s="32"/>
+    </row>
+    <row r="36" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="53"/>
+      <c r="B36" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="C35" s="9">
+      <c r="C36" s="9">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="D35" s="63" t="s">
+      <c r="D36" s="41" t="s">
         <v>65</v>
       </c>
-      <c r="E35" s="66"/>
-      <c r="F35" s="57"/>
-      <c r="G35" s="55"/>
-      <c r="H35" s="55"/>
-      <c r="I35" s="53"/>
-      <c r="J35" s="52"/>
-    </row>
-    <row r="36" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="26" t="s">
+      <c r="E36" s="44"/>
+      <c r="F36" s="37"/>
+      <c r="G36" s="35"/>
+      <c r="H36" s="35"/>
+      <c r="I36" s="33"/>
+      <c r="J36" s="32"/>
+    </row>
+    <row r="37" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="B36" s="60" t="s">
+      <c r="B37" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="C36" s="9">
+      <c r="C37" s="9">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="D36" s="63" t="s">
+      <c r="D37" s="41" t="s">
         <v>61</v>
       </c>
-      <c r="E36" s="66"/>
-      <c r="F36" s="57"/>
-      <c r="G36" s="55"/>
-      <c r="H36" s="55"/>
-      <c r="I36" s="54"/>
-      <c r="J36" s="58"/>
-    </row>
-    <row r="37" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="27"/>
-      <c r="B37" s="67"/>
-      <c r="C37" s="9">
+      <c r="E37" s="44"/>
+      <c r="F37" s="37"/>
+      <c r="G37" s="35"/>
+      <c r="H37" s="35"/>
+      <c r="I37" s="34"/>
+      <c r="J37" s="38"/>
+    </row>
+    <row r="38" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="49"/>
+      <c r="B38" s="51"/>
+      <c r="C38" s="9">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="D37" s="63" t="s">
+      <c r="D38" s="41" t="s">
         <v>62</v>
       </c>
-      <c r="E37" s="66"/>
-      <c r="F37" s="57"/>
-      <c r="G37" s="55"/>
-      <c r="H37" s="55"/>
-      <c r="I37" s="53"/>
-      <c r="J37" s="52"/>
-    </row>
-    <row r="38" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="27"/>
-      <c r="B38" s="61"/>
-      <c r="C38" s="9">
+      <c r="E38" s="44"/>
+      <c r="F38" s="37"/>
+      <c r="G38" s="35"/>
+      <c r="H38" s="35"/>
+      <c r="I38" s="33"/>
+      <c r="J38" s="32"/>
+    </row>
+    <row r="39" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="49"/>
+      <c r="B39" s="52"/>
+      <c r="C39" s="9">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="D38" s="63" t="s">
+      <c r="D39" s="41" t="s">
         <v>64</v>
       </c>
-      <c r="E38" s="66"/>
-      <c r="F38" s="57"/>
-      <c r="G38" s="55"/>
-      <c r="H38" s="55"/>
-      <c r="I38" s="54"/>
-      <c r="J38" s="58"/>
-    </row>
-    <row r="39" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="17"/>
-      <c r="B39" s="68" t="s">
+      <c r="E39" s="44"/>
+      <c r="F39" s="37"/>
+      <c r="G39" s="35"/>
+      <c r="H39" s="35"/>
+      <c r="I39" s="34"/>
+      <c r="J39" s="38"/>
+    </row>
+    <row r="40" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="53"/>
+      <c r="B40" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="C39" s="9">
+      <c r="C40" s="9">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="D39" s="63" t="s">
+      <c r="D40" s="41" t="s">
         <v>65</v>
       </c>
-      <c r="E39" s="66"/>
-      <c r="F39" s="57"/>
-      <c r="G39" s="55"/>
-      <c r="H39" s="55"/>
-      <c r="I39" s="55"/>
-      <c r="J39" s="58"/>
-    </row>
-    <row r="40" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="26" t="s">
+      <c r="E40" s="44"/>
+      <c r="F40" s="37"/>
+      <c r="G40" s="35"/>
+      <c r="H40" s="35"/>
+      <c r="I40" s="35"/>
+      <c r="J40" s="38"/>
+    </row>
+    <row r="41" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="48" t="s">
         <v>63</v>
       </c>
-      <c r="B40" s="60" t="s">
+      <c r="B41" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="C40" s="9">
+      <c r="C41" s="9">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="D40" s="62" t="s">
+      <c r="D41" s="40" t="s">
         <v>66</v>
       </c>
-      <c r="E40" s="65"/>
-      <c r="F40" s="56"/>
-      <c r="G40" s="54"/>
-      <c r="H40" s="54"/>
-      <c r="I40" s="53"/>
-      <c r="J40" s="52"/>
-    </row>
-    <row r="41" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="28"/>
-      <c r="B41" s="69"/>
-      <c r="C41" s="9">
+      <c r="E41" s="43"/>
+      <c r="F41" s="36"/>
+      <c r="G41" s="34"/>
+      <c r="H41" s="34"/>
+      <c r="I41" s="33"/>
+      <c r="J41" s="32"/>
+    </row>
+    <row r="42" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="53"/>
+      <c r="B42" s="54"/>
+      <c r="C42" s="9">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-      <c r="D41" s="63" t="s">
+      <c r="D42" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="E41" s="66"/>
-      <c r="F41" s="57"/>
-      <c r="G41" s="55"/>
-      <c r="H41" s="55"/>
-      <c r="I41" s="53"/>
-      <c r="J41" s="52"/>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E46" s="51"/>
+      <c r="E42" s="44"/>
+      <c r="F42" s="37"/>
+      <c r="G42" s="35"/>
+      <c r="H42" s="35"/>
+      <c r="I42" s="33"/>
+      <c r="J42" s="32"/>
+    </row>
+    <row r="43" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="48" t="s">
+        <v>71</v>
+      </c>
+      <c r="B43" s="80" t="s">
+        <v>9</v>
+      </c>
+      <c r="C43" s="9">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="D43" s="41" t="s">
+        <v>75</v>
+      </c>
+      <c r="E43" s="44"/>
+      <c r="F43" s="37"/>
+      <c r="G43" s="35"/>
+      <c r="H43" s="35"/>
+      <c r="I43" s="33"/>
+      <c r="J43" s="32"/>
+    </row>
+    <row r="44" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="49"/>
+      <c r="B44" s="51"/>
+      <c r="C44" s="9">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="D44" s="41" t="s">
+        <v>79</v>
+      </c>
+      <c r="E44" s="44"/>
+      <c r="F44" s="37"/>
+      <c r="G44" s="35"/>
+      <c r="H44" s="35"/>
+      <c r="I44" s="33"/>
+      <c r="J44" s="32"/>
+    </row>
+    <row r="45" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="49"/>
+      <c r="B45" s="51"/>
+      <c r="C45" s="9">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="D45" s="41" t="s">
+        <v>80</v>
+      </c>
+      <c r="E45" s="44"/>
+      <c r="F45" s="37"/>
+      <c r="G45" s="35"/>
+      <c r="H45" s="35"/>
+      <c r="I45" s="33"/>
+      <c r="J45" s="32"/>
+    </row>
+    <row r="46" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="49"/>
+      <c r="B46" s="54"/>
+      <c r="C46" s="9">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="D46" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="E46" s="44"/>
+      <c r="F46" s="37"/>
+      <c r="G46" s="35"/>
+      <c r="H46" s="35"/>
+      <c r="I46" s="33"/>
+      <c r="J46" s="32"/>
+    </row>
+    <row r="47" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="53"/>
+      <c r="B47" s="46" t="s">
+        <v>25</v>
+      </c>
+      <c r="C47" s="9">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="D47" s="41"/>
+      <c r="E47" s="44"/>
+      <c r="F47" s="37"/>
+      <c r="G47" s="35"/>
+      <c r="H47" s="35"/>
+      <c r="I47" s="33"/>
+      <c r="J47" s="32"/>
+    </row>
+    <row r="48" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="48" t="s">
+        <v>72</v>
+      </c>
+      <c r="B48" s="80" t="s">
+        <v>9</v>
+      </c>
+      <c r="C48" s="9">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="D48" s="41" t="s">
+        <v>77</v>
+      </c>
+      <c r="E48" s="44"/>
+      <c r="F48" s="37"/>
+      <c r="G48" s="35"/>
+      <c r="H48" s="35"/>
+      <c r="I48" s="33"/>
+      <c r="J48" s="32"/>
+    </row>
+    <row r="49" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="49"/>
+      <c r="B49" s="54"/>
+      <c r="C49" s="9">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="D49" s="41" t="s">
+        <v>78</v>
+      </c>
+      <c r="E49" s="44"/>
+      <c r="F49" s="37"/>
+      <c r="G49" s="35"/>
+      <c r="H49" s="35"/>
+      <c r="I49" s="33"/>
+      <c r="J49" s="32"/>
+    </row>
+    <row r="50" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="49"/>
+      <c r="B50" s="46" t="s">
+        <v>25</v>
+      </c>
+      <c r="C50" s="9">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="D50" s="41" t="s">
+        <v>81</v>
+      </c>
+      <c r="E50" s="44"/>
+      <c r="F50" s="37"/>
+      <c r="G50" s="35"/>
+      <c r="H50" s="35"/>
+      <c r="I50" s="33"/>
+      <c r="J50" s="32"/>
+    </row>
+    <row r="51" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="53"/>
+      <c r="B51" s="81"/>
+      <c r="C51" s="9">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="D51" s="41"/>
+      <c r="E51" s="44"/>
+      <c r="F51" s="37"/>
+      <c r="G51" s="35"/>
+      <c r="H51" s="35"/>
+      <c r="I51" s="33"/>
+      <c r="J51" s="32"/>
     </row>
   </sheetData>
-  <mergeCells count="24">
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="A36:A38"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="A40:A41"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="A15:A20"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="A24:A26"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="A27:A29"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="A30:A32"/>
-    <mergeCell ref="B30:B32"/>
-    <mergeCell ref="B15:B18"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="B3:B8"/>
-    <mergeCell ref="A3:A8"/>
-    <mergeCell ref="A9:A14"/>
-    <mergeCell ref="B9:B12"/>
-    <mergeCell ref="B13:B14"/>
+  <mergeCells count="30">
+    <mergeCell ref="A48:A51"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="A43:A47"/>
+    <mergeCell ref="E1:F2"/>
+    <mergeCell ref="G1:I2"/>
+    <mergeCell ref="A1:D2"/>
+    <mergeCell ref="B43:B46"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="B4:B9"/>
+    <mergeCell ref="A4:A9"/>
+    <mergeCell ref="A10:A15"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="B31:B33"/>
+    <mergeCell ref="B16:B19"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="A16:A21"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="B37:B39"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="A37:A40"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
[ATUALIZAÇÃO] - Art 17.
</commit_message>
<xml_diff>
--- a/Documentation/17-Analise_dos_Eventos_para_cada_Cenario.xlsx
+++ b/Documentation/17-Analise_dos_Eventos_para_cada_Cenario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/eed59d4ebf12600b/Documentos/Projeto/Faculdade/Silpan/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="306" documentId="8_{76FC5D5F-DBAD-408C-BCAE-F93491C61B30}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{DB71B1B2-66BF-43FA-B25E-161F7C840BC8}"/>
+  <xr:revisionPtr revIDLastSave="375" documentId="8_{76FC5D5F-DBAD-408C-BCAE-F93491C61B30}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{04698456-6EAA-4A53-8ED9-BF343C80AE74}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="95">
   <si>
     <t>Capacidades</t>
   </si>
@@ -319,6 +319,45 @@
   </si>
   <si>
     <t>Fabricantte não entrega produtos</t>
+  </si>
+  <si>
+    <t>x(20, 23, 26)</t>
+  </si>
+  <si>
+    <t>x(29)</t>
+  </si>
+  <si>
+    <t>x(30)</t>
+  </si>
+  <si>
+    <t>x(31)</t>
+  </si>
+  <si>
+    <t>x(34)</t>
+  </si>
+  <si>
+    <t>x(35)</t>
+  </si>
+  <si>
+    <t>x(32)</t>
+  </si>
+  <si>
+    <t>x(38)</t>
+  </si>
+  <si>
+    <t>x(40)</t>
+  </si>
+  <si>
+    <t>x(41)</t>
+  </si>
+  <si>
+    <t>x(42)</t>
+  </si>
+  <si>
+    <t>x(43)</t>
+  </si>
+  <si>
+    <t>x(44)</t>
   </si>
 </sst>
 </file>
@@ -379,7 +418,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -410,6 +449,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="39">
     <border>
@@ -893,7 +938,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1029,110 +1074,113 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1448,10 +1496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J51"/>
+  <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34:A36"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1460,59 +1508,60 @@
     <col min="4" max="4" width="52.28515625" customWidth="1"/>
     <col min="5" max="5" width="12.5703125" customWidth="1"/>
     <col min="6" max="6" width="10.7109375" customWidth="1"/>
+    <col min="7" max="7" width="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="70"/>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="78" t="s">
+      <c r="A1" s="61"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="53" t="s">
         <v>73</v>
       </c>
-      <c r="F1" s="79"/>
-      <c r="G1" s="72" t="s">
+      <c r="F1" s="54"/>
+      <c r="G1" s="57" t="s">
         <v>74</v>
       </c>
-      <c r="H1" s="76"/>
-      <c r="I1" s="73"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="59"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="69"/>
-      <c r="B2" s="69"/>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="74"/>
-      <c r="F2" s="75"/>
-      <c r="G2" s="74"/>
-      <c r="H2" s="77"/>
-      <c r="I2" s="75"/>
+      <c r="A2" s="62"/>
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="56"/>
       <c r="J2" s="18"/>
     </row>
     <row r="3" spans="1:10" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="59" t="s">
+      <c r="A3" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="60"/>
+      <c r="B3" s="65"/>
       <c r="C3" s="8" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="71" t="s">
+      <c r="E3" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="71" t="s">
+      <c r="F3" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="71" t="s">
+      <c r="G3" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="71" t="s">
+      <c r="H3" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="71" t="s">
+      <c r="I3" s="47" t="s">
         <v>7</v>
       </c>
       <c r="J3" s="2" t="s">
@@ -1523,7 +1572,7 @@
       <c r="A4" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="57" t="s">
+      <c r="B4" s="66" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="9">
@@ -1543,7 +1592,7 @@
     </row>
     <row r="5" spans="1:10" ht="16.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="49"/>
-      <c r="B5" s="58"/>
+      <c r="B5" s="67"/>
       <c r="C5" s="10">
         <f>C4+1</f>
         <v>2</v>
@@ -1562,9 +1611,9 @@
     </row>
     <row r="6" spans="1:10" ht="16.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="49"/>
-      <c r="B6" s="58"/>
+      <c r="B6" s="67"/>
       <c r="C6" s="10">
-        <f t="shared" ref="C6:C51" si="0">C5+1</f>
+        <f t="shared" ref="C6:C49" si="0">C5+1</f>
         <v>3</v>
       </c>
       <c r="D6" s="7" t="s">
@@ -1581,7 +1630,7 @@
     </row>
     <row r="7" spans="1:10" ht="16.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="49"/>
-      <c r="B7" s="58"/>
+      <c r="B7" s="67"/>
       <c r="C7" s="10">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1600,7 +1649,7 @@
     </row>
     <row r="8" spans="1:10" ht="16.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="49"/>
-      <c r="B8" s="58"/>
+      <c r="B8" s="67"/>
       <c r="C8" s="10">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1618,8 +1667,8 @@
       <c r="J8" s="6"/>
     </row>
     <row r="9" spans="1:10" ht="16.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="53"/>
-      <c r="B9" s="61"/>
+      <c r="A9" s="50"/>
+      <c r="B9" s="68"/>
       <c r="C9" s="10">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1637,10 +1686,10 @@
       <c r="J9" s="6"/>
     </row>
     <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="62" t="s">
+      <c r="A10" s="69" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="65" t="s">
+      <c r="B10" s="72" t="s">
         <v>9</v>
       </c>
       <c r="C10" s="10">
@@ -1660,8 +1709,8 @@
       <c r="J10" s="14"/>
     </row>
     <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="63"/>
-      <c r="B11" s="66"/>
+      <c r="A11" s="70"/>
+      <c r="B11" s="73"/>
       <c r="C11" s="10">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1679,8 +1728,8 @@
       <c r="J11" s="6"/>
     </row>
     <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="63"/>
-      <c r="B12" s="66"/>
+      <c r="A12" s="70"/>
+      <c r="B12" s="73"/>
       <c r="C12" s="10">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1698,8 +1747,8 @@
       <c r="J12" s="6"/>
     </row>
     <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="63"/>
-      <c r="B13" s="66"/>
+      <c r="A13" s="70"/>
+      <c r="B13" s="73"/>
       <c r="C13" s="10">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1717,8 +1766,8 @@
       <c r="J13" s="6"/>
     </row>
     <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="64"/>
-      <c r="B14" s="67" t="s">
+      <c r="A14" s="71"/>
+      <c r="B14" s="74" t="s">
         <v>25</v>
       </c>
       <c r="C14" s="10">
@@ -1738,8 +1787,8 @@
       <c r="J14" s="14"/>
     </row>
     <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="64"/>
-      <c r="B15" s="68"/>
+      <c r="A15" s="71"/>
+      <c r="B15" s="75"/>
       <c r="C15" s="24">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1760,7 +1809,7 @@
       <c r="A16" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="57" t="s">
+      <c r="B16" s="66" t="s">
         <v>9</v>
       </c>
       <c r="C16" s="9">
@@ -1781,7 +1830,7 @@
     </row>
     <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="49"/>
-      <c r="B17" s="58"/>
+      <c r="B17" s="67"/>
       <c r="C17" s="10">
         <f>C16+1</f>
         <v>14</v>
@@ -1800,7 +1849,7 @@
     </row>
     <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="49"/>
-      <c r="B18" s="58"/>
+      <c r="B18" s="67"/>
       <c r="C18" s="10">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1819,7 +1868,7 @@
     </row>
     <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="49"/>
-      <c r="B19" s="58"/>
+      <c r="B19" s="67"/>
       <c r="C19" s="9">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1838,7 +1887,7 @@
     </row>
     <row r="20" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="49"/>
-      <c r="B20" s="55" t="s">
+      <c r="B20" s="78" t="s">
         <v>25</v>
       </c>
       <c r="C20" s="10">
@@ -1859,7 +1908,7 @@
     </row>
     <row r="21" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="49"/>
-      <c r="B21" s="56"/>
+      <c r="B21" s="79"/>
       <c r="C21" s="10">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1880,7 +1929,7 @@
       <c r="A22" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="B22" s="50" t="s">
+      <c r="B22" s="76" t="s">
         <v>9</v>
       </c>
       <c r="C22" s="9">
@@ -1901,7 +1950,7 @@
     </row>
     <row r="23" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="49"/>
-      <c r="B23" s="52"/>
+      <c r="B23" s="77"/>
       <c r="C23" s="10">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1930,9 +1979,9 @@
       <c r="D24" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="E24" s="44"/>
-      <c r="F24" s="47" t="s">
-        <v>69</v>
+      <c r="E24" s="81"/>
+      <c r="F24" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="G24" s="35"/>
       <c r="H24" s="35"/>
@@ -1943,7 +1992,7 @@
       <c r="A25" s="48" t="s">
         <v>52</v>
       </c>
-      <c r="B25" s="50" t="s">
+      <c r="B25" s="76" t="s">
         <v>9</v>
       </c>
       <c r="C25" s="9">
@@ -1964,7 +2013,7 @@
     </row>
     <row r="26" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="49"/>
-      <c r="B26" s="52"/>
+      <c r="B26" s="77"/>
       <c r="C26" s="10">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -1993,9 +2042,9 @@
       <c r="D27" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="E27" s="44"/>
-      <c r="F27" s="47" t="s">
-        <v>69</v>
+      <c r="E27" s="81"/>
+      <c r="F27" s="82" t="s">
+        <v>11</v>
       </c>
       <c r="G27" s="35"/>
       <c r="H27" s="35"/>
@@ -2006,7 +2055,7 @@
       <c r="A28" s="48" t="s">
         <v>55</v>
       </c>
-      <c r="B28" s="50" t="s">
+      <c r="B28" s="76" t="s">
         <v>9</v>
       </c>
       <c r="C28" s="9">
@@ -2027,7 +2076,7 @@
     </row>
     <row r="29" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="49"/>
-      <c r="B29" s="52"/>
+      <c r="B29" s="77"/>
       <c r="C29" s="9">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -2056,9 +2105,9 @@
       <c r="D30" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="E30" s="44"/>
-      <c r="F30" s="47" t="s">
-        <v>69</v>
+      <c r="E30" s="81"/>
+      <c r="F30" s="82" t="s">
+        <v>11</v>
       </c>
       <c r="G30" s="35"/>
       <c r="H30" s="35"/>
@@ -2069,7 +2118,7 @@
       <c r="A31" s="48" t="s">
         <v>57</v>
       </c>
-      <c r="B31" s="50" t="s">
+      <c r="B31" s="76" t="s">
         <v>9</v>
       </c>
       <c r="C31" s="9">
@@ -2082,7 +2131,7 @@
       <c r="E31" s="43"/>
       <c r="F31" s="36"/>
       <c r="G31" s="34" t="s">
-        <v>11</v>
+        <v>82</v>
       </c>
       <c r="H31" s="34"/>
       <c r="I31" s="33"/>
@@ -2090,7 +2139,7 @@
     </row>
     <row r="32" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="49"/>
-      <c r="B32" s="51"/>
+      <c r="B32" s="63"/>
       <c r="C32" s="9">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -2100,14 +2149,16 @@
       </c>
       <c r="E32" s="44"/>
       <c r="F32" s="37"/>
-      <c r="G32" s="35"/>
+      <c r="G32" s="35" t="s">
+        <v>83</v>
+      </c>
       <c r="H32" s="35"/>
       <c r="I32" s="33"/>
       <c r="J32" s="32"/>
     </row>
     <row r="33" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="49"/>
-      <c r="B33" s="52"/>
+      <c r="B33" s="77"/>
       <c r="C33" s="9">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -2117,7 +2168,9 @@
       </c>
       <c r="E33" s="44"/>
       <c r="F33" s="37"/>
-      <c r="G33" s="35"/>
+      <c r="G33" s="35" t="s">
+        <v>84</v>
+      </c>
       <c r="H33" s="35"/>
       <c r="I33" s="34"/>
       <c r="J33" s="38"/>
@@ -2126,7 +2179,7 @@
       <c r="A34" s="48" t="s">
         <v>58</v>
       </c>
-      <c r="B34" s="50" t="s">
+      <c r="B34" s="76" t="s">
         <v>9</v>
       </c>
       <c r="C34" s="9">
@@ -2136,7 +2189,9 @@
       <c r="D34" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="E34" s="43"/>
+      <c r="E34" s="43" t="s">
+        <v>84</v>
+      </c>
       <c r="F34" s="36"/>
       <c r="G34" s="34"/>
       <c r="H34" s="34"/>
@@ -2145,7 +2200,7 @@
     </row>
     <row r="35" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="49"/>
-      <c r="B35" s="51"/>
+      <c r="B35" s="63"/>
       <c r="C35" s="9">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -2153,7 +2208,9 @@
       <c r="D35" s="41" t="s">
         <v>62</v>
       </c>
-      <c r="E35" s="44"/>
+      <c r="E35" s="44" t="s">
+        <v>85</v>
+      </c>
       <c r="F35" s="37"/>
       <c r="G35" s="35"/>
       <c r="H35" s="35"/>
@@ -2161,7 +2218,7 @@
       <c r="J35" s="32"/>
     </row>
     <row r="36" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="53"/>
+      <c r="A36" s="50"/>
       <c r="B36" s="39" t="s">
         <v>25</v>
       </c>
@@ -2173,7 +2230,9 @@
         <v>65</v>
       </c>
       <c r="E36" s="44"/>
-      <c r="F36" s="37"/>
+      <c r="F36" s="37" t="s">
+        <v>11</v>
+      </c>
       <c r="G36" s="35"/>
       <c r="H36" s="35"/>
       <c r="I36" s="33"/>
@@ -2183,7 +2242,7 @@
       <c r="A37" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="B37" s="50" t="s">
+      <c r="B37" s="76" t="s">
         <v>9</v>
       </c>
       <c r="C37" s="9">
@@ -2193,7 +2252,9 @@
       <c r="D37" s="41" t="s">
         <v>61</v>
       </c>
-      <c r="E37" s="44"/>
+      <c r="E37" s="43" t="s">
+        <v>84</v>
+      </c>
       <c r="F37" s="37"/>
       <c r="G37" s="35"/>
       <c r="H37" s="35"/>
@@ -2202,7 +2263,7 @@
     </row>
     <row r="38" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="49"/>
-      <c r="B38" s="51"/>
+      <c r="B38" s="63"/>
       <c r="C38" s="9">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -2210,7 +2271,9 @@
       <c r="D38" s="41" t="s">
         <v>62</v>
       </c>
-      <c r="E38" s="44"/>
+      <c r="E38" s="43" t="s">
+        <v>86</v>
+      </c>
       <c r="F38" s="37"/>
       <c r="G38" s="35"/>
       <c r="H38" s="35"/>
@@ -2219,7 +2282,7 @@
     </row>
     <row r="39" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="49"/>
-      <c r="B39" s="52"/>
+      <c r="B39" s="77"/>
       <c r="C39" s="9">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -2227,7 +2290,9 @@
       <c r="D39" s="41" t="s">
         <v>64</v>
       </c>
-      <c r="E39" s="44"/>
+      <c r="E39" s="43" t="s">
+        <v>87</v>
+      </c>
       <c r="F39" s="37"/>
       <c r="G39" s="35"/>
       <c r="H39" s="35"/>
@@ -2235,7 +2300,7 @@
       <c r="J39" s="38"/>
     </row>
     <row r="40" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="53"/>
+      <c r="A40" s="50"/>
       <c r="B40" s="45" t="s">
         <v>25</v>
       </c>
@@ -2247,7 +2312,9 @@
         <v>65</v>
       </c>
       <c r="E40" s="44"/>
-      <c r="F40" s="37"/>
+      <c r="F40" s="37" t="s">
+        <v>11</v>
+      </c>
       <c r="G40" s="35"/>
       <c r="H40" s="35"/>
       <c r="I40" s="35"/>
@@ -2257,7 +2324,7 @@
       <c r="A41" s="48" t="s">
         <v>63</v>
       </c>
-      <c r="B41" s="50" t="s">
+      <c r="B41" s="76" t="s">
         <v>9</v>
       </c>
       <c r="C41" s="9">
@@ -2267,7 +2334,9 @@
       <c r="D41" s="40" t="s">
         <v>66</v>
       </c>
-      <c r="E41" s="43"/>
+      <c r="E41" s="43" t="s">
+        <v>88</v>
+      </c>
       <c r="F41" s="36"/>
       <c r="G41" s="34"/>
       <c r="H41" s="34"/>
@@ -2275,8 +2344,8 @@
       <c r="J41" s="32"/>
     </row>
     <row r="42" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="53"/>
-      <c r="B42" s="54"/>
+      <c r="A42" s="50"/>
+      <c r="B42" s="52"/>
       <c r="C42" s="9">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -2284,7 +2353,9 @@
       <c r="D42" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="E42" s="44"/>
+      <c r="E42" s="44" t="s">
+        <v>89</v>
+      </c>
       <c r="F42" s="37"/>
       <c r="G42" s="35"/>
       <c r="H42" s="35"/>
@@ -2295,14 +2366,14 @@
       <c r="A43" s="48" t="s">
         <v>71</v>
       </c>
-      <c r="B43" s="80" t="s">
+      <c r="B43" s="51" t="s">
         <v>9</v>
       </c>
       <c r="C43" s="9">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="D43" s="41" t="s">
+      <c r="D43" s="80" t="s">
         <v>75</v>
       </c>
       <c r="E43" s="44"/>
@@ -2310,19 +2381,23 @@
       <c r="G43" s="35"/>
       <c r="H43" s="35"/>
       <c r="I43" s="33"/>
-      <c r="J43" s="32"/>
+      <c r="J43" s="32" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="44" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="49"/>
-      <c r="B44" s="51"/>
+      <c r="B44" s="63"/>
       <c r="C44" s="9">
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
-      <c r="D44" s="41" t="s">
+      <c r="D44" s="80" t="s">
         <v>79</v>
       </c>
-      <c r="E44" s="44"/>
+      <c r="E44" s="44" t="s">
+        <v>90</v>
+      </c>
       <c r="F44" s="37"/>
       <c r="G44" s="35"/>
       <c r="H44" s="35"/>
@@ -2331,132 +2406,124 @@
     </row>
     <row r="45" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="49"/>
-      <c r="B45" s="51"/>
+      <c r="B45" s="63"/>
       <c r="C45" s="9">
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
-      <c r="D45" s="41" t="s">
+      <c r="D45" s="80" t="s">
         <v>80</v>
       </c>
       <c r="E45" s="44"/>
       <c r="F45" s="37"/>
-      <c r="G45" s="35"/>
+      <c r="G45" s="35" t="s">
+        <v>91</v>
+      </c>
       <c r="H45" s="35"/>
       <c r="I45" s="33"/>
       <c r="J45" s="32"/>
     </row>
     <row r="46" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="49"/>
-      <c r="B46" s="54"/>
+      <c r="B46" s="52"/>
       <c r="C46" s="9">
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
-      <c r="D46" s="41" t="s">
+      <c r="D46" s="80" t="s">
         <v>76</v>
       </c>
       <c r="E46" s="44"/>
       <c r="F46" s="37"/>
-      <c r="G46" s="35"/>
+      <c r="G46" s="35" t="s">
+        <v>92</v>
+      </c>
       <c r="H46" s="35"/>
       <c r="I46" s="33"/>
       <c r="J46" s="32"/>
     </row>
-    <row r="47" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="53"/>
-      <c r="B47" s="46" t="s">
-        <v>25</v>
+    <row r="47" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="48" t="s">
+        <v>72</v>
+      </c>
+      <c r="B47" s="51" t="s">
+        <v>9</v>
       </c>
       <c r="C47" s="9">
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
-      <c r="D47" s="41"/>
-      <c r="E47" s="44"/>
+      <c r="D47" s="80" t="s">
+        <v>77</v>
+      </c>
+      <c r="E47" s="44" t="s">
+        <v>93</v>
+      </c>
       <c r="F47" s="37"/>
       <c r="G47" s="35"/>
       <c r="H47" s="35"/>
       <c r="I47" s="33"/>
       <c r="J47" s="32"/>
     </row>
-    <row r="48" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="48" t="s">
-        <v>72</v>
-      </c>
-      <c r="B48" s="80" t="s">
-        <v>9</v>
-      </c>
+    <row r="48" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="49"/>
+      <c r="B48" s="52"/>
       <c r="C48" s="9">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-      <c r="D48" s="41" t="s">
-        <v>77</v>
+      <c r="D48" s="80" t="s">
+        <v>78</v>
       </c>
       <c r="E48" s="44"/>
       <c r="F48" s="37"/>
-      <c r="G48" s="35"/>
+      <c r="G48" s="35" t="s">
+        <v>94</v>
+      </c>
       <c r="H48" s="35"/>
       <c r="I48" s="33"/>
       <c r="J48" s="32"/>
     </row>
     <row r="49" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="49"/>
-      <c r="B49" s="54"/>
+      <c r="B49" s="46" t="s">
+        <v>25</v>
+      </c>
       <c r="C49" s="9">
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
-      <c r="D49" s="41" t="s">
-        <v>78</v>
+      <c r="D49" s="80" t="s">
+        <v>81</v>
       </c>
       <c r="E49" s="44"/>
-      <c r="F49" s="37"/>
+      <c r="F49" s="37" t="s">
+        <v>11</v>
+      </c>
       <c r="G49" s="35"/>
       <c r="H49" s="35"/>
       <c r="I49" s="33"/>
       <c r="J49" s="32"/>
     </row>
-    <row r="50" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="49"/>
-      <c r="B50" s="46" t="s">
-        <v>25</v>
-      </c>
-      <c r="C50" s="9">
-        <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="D50" s="41" t="s">
-        <v>81</v>
-      </c>
-      <c r="E50" s="44"/>
-      <c r="F50" s="37"/>
-      <c r="G50" s="35"/>
-      <c r="H50" s="35"/>
-      <c r="I50" s="33"/>
-      <c r="J50" s="32"/>
-    </row>
-    <row r="51" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="53"/>
-      <c r="B51" s="81"/>
-      <c r="C51" s="9">
-        <f t="shared" si="0"/>
-        <v>48</v>
-      </c>
-      <c r="D51" s="41"/>
-      <c r="E51" s="44"/>
-      <c r="F51" s="37"/>
-      <c r="G51" s="35"/>
-      <c r="H51" s="35"/>
-      <c r="I51" s="33"/>
-      <c r="J51" s="32"/>
-    </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="A48:A51"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="A43:A47"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="B37:B39"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="A37:A40"/>
+    <mergeCell ref="B31:B33"/>
+    <mergeCell ref="B16:B19"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="A16:A21"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="A47:A49"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="A43:A46"/>
     <mergeCell ref="E1:F2"/>
     <mergeCell ref="G1:I2"/>
     <mergeCell ref="A1:D2"/>
@@ -2470,20 +2537,6 @@
     <mergeCell ref="A28:A30"/>
     <mergeCell ref="B28:B29"/>
     <mergeCell ref="A31:A33"/>
-    <mergeCell ref="B31:B33"/>
-    <mergeCell ref="B16:B19"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="A16:A21"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="A22:A24"/>
-    <mergeCell ref="A25:A27"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="B37:B39"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="A34:A36"/>
-    <mergeCell ref="A37:A40"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
[Criado] Art 16. - DFD tratar pagamentos
</commit_message>
<xml_diff>
--- a/Documentation/17-Analise_dos_Eventos_para_cada_Cenario.xlsx
+++ b/Documentation/17-Analise_dos_Eventos_para_cada_Cenario.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/eed59d4ebf12600b/Documentos/Projeto/Faculdade/Silpan/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="375" documentId="8_{76FC5D5F-DBAD-408C-BCAE-F93491C61B30}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{04698456-6EAA-4A53-8ED9-BF343C80AE74}"/>
+  <xr:revisionPtr revIDLastSave="378" documentId="8_{76FC5D5F-DBAD-408C-BCAE-F93491C61B30}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{FC9C34CB-46AE-4374-908D-145CEFBCA4C6}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16320" yWindow="-8580" windowWidth="16440" windowHeight="38190" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DFD Orçamento sob medida" sheetId="5" r:id="rId1"/>
@@ -364,7 +364,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -417,6 +417,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -938,7 +946,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1077,13 +1085,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1140,6 +1154,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1173,15 +1190,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1496,10 +1505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J49"/>
+  <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" topLeftCell="B7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1512,37 +1521,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="61"/>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="53" t="s">
+      <c r="A1" s="63"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="55" t="s">
         <v>73</v>
       </c>
-      <c r="F1" s="54"/>
-      <c r="G1" s="57" t="s">
+      <c r="F1" s="56"/>
+      <c r="G1" s="59" t="s">
         <v>74</v>
       </c>
-      <c r="H1" s="58"/>
-      <c r="I1" s="59"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="61"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="62"/>
-      <c r="B2" s="62"/>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="60"/>
-      <c r="I2" s="56"/>
+      <c r="A2" s="64"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="58"/>
       <c r="J2" s="18"/>
     </row>
     <row r="3" spans="1:10" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="64" t="s">
+      <c r="A3" s="66" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="65"/>
+      <c r="B3" s="67"/>
       <c r="C3" s="8" t="s">
         <v>1</v>
       </c>
@@ -1569,10 +1578,10 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="16.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="48" t="s">
+      <c r="A4" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="66" t="s">
+      <c r="B4" s="68" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="9">
@@ -1591,8 +1600,8 @@
       <c r="J4" s="6"/>
     </row>
     <row r="5" spans="1:10" ht="16.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="49"/>
-      <c r="B5" s="67"/>
+      <c r="A5" s="52"/>
+      <c r="B5" s="69"/>
       <c r="C5" s="10">
         <f>C4+1</f>
         <v>2</v>
@@ -1610,8 +1619,8 @@
       <c r="J5" s="6"/>
     </row>
     <row r="6" spans="1:10" ht="16.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="49"/>
-      <c r="B6" s="67"/>
+      <c r="A6" s="52"/>
+      <c r="B6" s="69"/>
       <c r="C6" s="10">
         <f t="shared" ref="C6:C49" si="0">C5+1</f>
         <v>3</v>
@@ -1629,8 +1638,8 @@
       <c r="J6" s="6"/>
     </row>
     <row r="7" spans="1:10" ht="16.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="49"/>
-      <c r="B7" s="67"/>
+      <c r="A7" s="52"/>
+      <c r="B7" s="69"/>
       <c r="C7" s="10">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1648,8 +1657,8 @@
       <c r="J7" s="6"/>
     </row>
     <row r="8" spans="1:10" ht="16.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="49"/>
-      <c r="B8" s="67"/>
+      <c r="A8" s="52"/>
+      <c r="B8" s="69"/>
       <c r="C8" s="10">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1667,8 +1676,8 @@
       <c r="J8" s="6"/>
     </row>
     <row r="9" spans="1:10" ht="16.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="50"/>
-      <c r="B9" s="68"/>
+      <c r="A9" s="71"/>
+      <c r="B9" s="70"/>
       <c r="C9" s="10">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1686,10 +1695,10 @@
       <c r="J9" s="6"/>
     </row>
     <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="69" t="s">
+      <c r="A10" s="72" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="72" t="s">
+      <c r="B10" s="75" t="s">
         <v>9</v>
       </c>
       <c r="C10" s="10">
@@ -1709,8 +1718,8 @@
       <c r="J10" s="14"/>
     </row>
     <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="70"/>
-      <c r="B11" s="73"/>
+      <c r="A11" s="73"/>
+      <c r="B11" s="76"/>
       <c r="C11" s="10">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1728,8 +1737,8 @@
       <c r="J11" s="6"/>
     </row>
     <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="70"/>
-      <c r="B12" s="73"/>
+      <c r="A12" s="73"/>
+      <c r="B12" s="76"/>
       <c r="C12" s="10">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1747,8 +1756,8 @@
       <c r="J12" s="6"/>
     </row>
     <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="70"/>
-      <c r="B13" s="73"/>
+      <c r="A13" s="73"/>
+      <c r="B13" s="76"/>
       <c r="C13" s="10">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1766,8 +1775,8 @@
       <c r="J13" s="6"/>
     </row>
     <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="71"/>
-      <c r="B14" s="74" t="s">
+      <c r="A14" s="74"/>
+      <c r="B14" s="77" t="s">
         <v>25</v>
       </c>
       <c r="C14" s="10">
@@ -1787,8 +1796,8 @@
       <c r="J14" s="14"/>
     </row>
     <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="71"/>
-      <c r="B15" s="75"/>
+      <c r="A15" s="74"/>
+      <c r="B15" s="78"/>
       <c r="C15" s="24">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1806,10 +1815,10 @@
       <c r="J15" s="23"/>
     </row>
     <row r="16" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="48" t="s">
+      <c r="A16" s="51" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="66" t="s">
+      <c r="B16" s="68" t="s">
         <v>9</v>
       </c>
       <c r="C16" s="9">
@@ -1829,8 +1838,8 @@
       <c r="J16" s="29"/>
     </row>
     <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="49"/>
-      <c r="B17" s="67"/>
+      <c r="A17" s="52"/>
+      <c r="B17" s="69"/>
       <c r="C17" s="10">
         <f>C16+1</f>
         <v>14</v>
@@ -1848,8 +1857,8 @@
       <c r="J17" s="30"/>
     </row>
     <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="49"/>
-      <c r="B18" s="67"/>
+      <c r="A18" s="52"/>
+      <c r="B18" s="69"/>
       <c r="C18" s="10">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1867,8 +1876,8 @@
       <c r="J18" s="30"/>
     </row>
     <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="49"/>
-      <c r="B19" s="67"/>
+      <c r="A19" s="52"/>
+      <c r="B19" s="69"/>
       <c r="C19" s="9">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1886,8 +1895,8 @@
       <c r="J19" s="30"/>
     </row>
     <row r="20" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="49"/>
-      <c r="B20" s="78" t="s">
+      <c r="A20" s="52"/>
+      <c r="B20" s="81" t="s">
         <v>25</v>
       </c>
       <c r="C20" s="10">
@@ -1907,8 +1916,8 @@
       <c r="J20" s="30"/>
     </row>
     <row r="21" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="49"/>
-      <c r="B21" s="79"/>
+      <c r="A21" s="52"/>
+      <c r="B21" s="82"/>
       <c r="C21" s="10">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1926,10 +1935,10 @@
       <c r="J21" s="31"/>
     </row>
     <row r="22" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="48" t="s">
+      <c r="A22" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="B22" s="76" t="s">
+      <c r="B22" s="79" t="s">
         <v>9</v>
       </c>
       <c r="C22" s="9">
@@ -1949,8 +1958,8 @@
       <c r="J22" s="32"/>
     </row>
     <row r="23" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="49"/>
-      <c r="B23" s="77"/>
+      <c r="A23" s="52"/>
+      <c r="B23" s="80"/>
       <c r="C23" s="10">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1968,7 +1977,7 @@
       <c r="J23" s="38"/>
     </row>
     <row r="24" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="49"/>
+      <c r="A24" s="52"/>
       <c r="B24" s="39" t="s">
         <v>25</v>
       </c>
@@ -1979,7 +1988,7 @@
       <c r="D24" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="E24" s="81"/>
+      <c r="E24" s="49"/>
       <c r="F24" s="5" t="s">
         <v>11</v>
       </c>
@@ -1989,10 +1998,10 @@
       <c r="J24" s="38"/>
     </row>
     <row r="25" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="48" t="s">
+      <c r="A25" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="B25" s="76" t="s">
+      <c r="B25" s="79" t="s">
         <v>9</v>
       </c>
       <c r="C25" s="9">
@@ -2012,8 +2021,8 @@
       <c r="J25" s="32"/>
     </row>
     <row r="26" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="49"/>
-      <c r="B26" s="77"/>
+      <c r="A26" s="52"/>
+      <c r="B26" s="80"/>
       <c r="C26" s="10">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -2031,7 +2040,7 @@
       <c r="J26" s="38"/>
     </row>
     <row r="27" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="49"/>
+      <c r="A27" s="52"/>
       <c r="B27" s="39" t="s">
         <v>25</v>
       </c>
@@ -2042,8 +2051,8 @@
       <c r="D27" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="E27" s="81"/>
-      <c r="F27" s="82" t="s">
+      <c r="E27" s="49"/>
+      <c r="F27" s="50" t="s">
         <v>11</v>
       </c>
       <c r="G27" s="35"/>
@@ -2052,10 +2061,10 @@
       <c r="J27" s="38"/>
     </row>
     <row r="28" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="48" t="s">
+      <c r="A28" s="51" t="s">
         <v>55</v>
       </c>
-      <c r="B28" s="76" t="s">
+      <c r="B28" s="79" t="s">
         <v>9</v>
       </c>
       <c r="C28" s="9">
@@ -2075,8 +2084,8 @@
       <c r="J28" s="32"/>
     </row>
     <row r="29" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="49"/>
-      <c r="B29" s="77"/>
+      <c r="A29" s="52"/>
+      <c r="B29" s="80"/>
       <c r="C29" s="9">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -2094,7 +2103,7 @@
       <c r="J29" s="38"/>
     </row>
     <row r="30" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="49"/>
+      <c r="A30" s="52"/>
       <c r="B30" s="39" t="s">
         <v>25</v>
       </c>
@@ -2105,8 +2114,8 @@
       <c r="D30" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="E30" s="81"/>
-      <c r="F30" s="82" t="s">
+      <c r="E30" s="49"/>
+      <c r="F30" s="50" t="s">
         <v>11</v>
       </c>
       <c r="G30" s="35"/>
@@ -2115,10 +2124,10 @@
       <c r="J30" s="38"/>
     </row>
     <row r="31" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="48" t="s">
+      <c r="A31" s="51" t="s">
         <v>57</v>
       </c>
-      <c r="B31" s="76" t="s">
+      <c r="B31" s="79" t="s">
         <v>9</v>
       </c>
       <c r="C31" s="9">
@@ -2138,8 +2147,8 @@
       <c r="J31" s="32"/>
     </row>
     <row r="32" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="49"/>
-      <c r="B32" s="63"/>
+      <c r="A32" s="52"/>
+      <c r="B32" s="65"/>
       <c r="C32" s="9">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -2157,8 +2166,8 @@
       <c r="J32" s="32"/>
     </row>
     <row r="33" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="49"/>
-      <c r="B33" s="77"/>
+      <c r="A33" s="52"/>
+      <c r="B33" s="80"/>
       <c r="C33" s="9">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -2176,10 +2185,10 @@
       <c r="J33" s="38"/>
     </row>
     <row r="34" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="48" t="s">
+      <c r="A34" s="51" t="s">
         <v>58</v>
       </c>
-      <c r="B34" s="76" t="s">
+      <c r="B34" s="79" t="s">
         <v>9</v>
       </c>
       <c r="C34" s="9">
@@ -2199,8 +2208,8 @@
       <c r="J34" s="32"/>
     </row>
     <row r="35" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="49"/>
-      <c r="B35" s="63"/>
+      <c r="A35" s="52"/>
+      <c r="B35" s="65"/>
       <c r="C35" s="9">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -2218,7 +2227,7 @@
       <c r="J35" s="32"/>
     </row>
     <row r="36" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="50"/>
+      <c r="A36" s="71"/>
       <c r="B36" s="39" t="s">
         <v>25</v>
       </c>
@@ -2239,10 +2248,10 @@
       <c r="J36" s="32"/>
     </row>
     <row r="37" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="48" t="s">
+      <c r="A37" s="51" t="s">
         <v>59</v>
       </c>
-      <c r="B37" s="76" t="s">
+      <c r="B37" s="79" t="s">
         <v>9</v>
       </c>
       <c r="C37" s="9">
@@ -2262,8 +2271,8 @@
       <c r="J37" s="38"/>
     </row>
     <row r="38" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="49"/>
-      <c r="B38" s="63"/>
+      <c r="A38" s="52"/>
+      <c r="B38" s="65"/>
       <c r="C38" s="9">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -2281,8 +2290,8 @@
       <c r="J38" s="32"/>
     </row>
     <row r="39" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="49"/>
-      <c r="B39" s="77"/>
+      <c r="A39" s="52"/>
+      <c r="B39" s="80"/>
       <c r="C39" s="9">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -2300,7 +2309,7 @@
       <c r="J39" s="38"/>
     </row>
     <row r="40" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="50"/>
+      <c r="A40" s="71"/>
       <c r="B40" s="45" t="s">
         <v>25</v>
       </c>
@@ -2321,10 +2330,10 @@
       <c r="J40" s="38"/>
     </row>
     <row r="41" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="48" t="s">
+      <c r="A41" s="51" t="s">
         <v>63</v>
       </c>
-      <c r="B41" s="76" t="s">
+      <c r="B41" s="79" t="s">
         <v>9</v>
       </c>
       <c r="C41" s="9">
@@ -2344,8 +2353,8 @@
       <c r="J41" s="32"/>
     </row>
     <row r="42" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="50"/>
-      <c r="B42" s="52"/>
+      <c r="A42" s="71"/>
+      <c r="B42" s="54"/>
       <c r="C42" s="9">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -2363,17 +2372,17 @@
       <c r="J42" s="32"/>
     </row>
     <row r="43" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="48" t="s">
+      <c r="A43" s="51" t="s">
         <v>71</v>
       </c>
-      <c r="B43" s="51" t="s">
+      <c r="B43" s="53" t="s">
         <v>9</v>
       </c>
       <c r="C43" s="9">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="D43" s="80" t="s">
+      <c r="D43" s="48" t="s">
         <v>75</v>
       </c>
       <c r="E43" s="44"/>
@@ -2386,13 +2395,13 @@
       </c>
     </row>
     <row r="44" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="49"/>
-      <c r="B44" s="63"/>
+      <c r="A44" s="52"/>
+      <c r="B44" s="65"/>
       <c r="C44" s="9">
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
-      <c r="D44" s="80" t="s">
+      <c r="D44" s="48" t="s">
         <v>79</v>
       </c>
       <c r="E44" s="44" t="s">
@@ -2405,13 +2414,13 @@
       <c r="J44" s="32"/>
     </row>
     <row r="45" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="49"/>
-      <c r="B45" s="63"/>
+      <c r="A45" s="52"/>
+      <c r="B45" s="65"/>
       <c r="C45" s="9">
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
-      <c r="D45" s="80" t="s">
+      <c r="D45" s="48" t="s">
         <v>80</v>
       </c>
       <c r="E45" s="44"/>
@@ -2424,13 +2433,13 @@
       <c r="J45" s="32"/>
     </row>
     <row r="46" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="49"/>
-      <c r="B46" s="52"/>
+      <c r="A46" s="52"/>
+      <c r="B46" s="54"/>
       <c r="C46" s="9">
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
-      <c r="D46" s="80" t="s">
+      <c r="D46" s="48" t="s">
         <v>76</v>
       </c>
       <c r="E46" s="44"/>
@@ -2443,17 +2452,17 @@
       <c r="J46" s="32"/>
     </row>
     <row r="47" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="48" t="s">
+      <c r="A47" s="51" t="s">
         <v>72</v>
       </c>
-      <c r="B47" s="51" t="s">
+      <c r="B47" s="53" t="s">
         <v>9</v>
       </c>
       <c r="C47" s="9">
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
-      <c r="D47" s="80" t="s">
+      <c r="D47" s="48" t="s">
         <v>77</v>
       </c>
       <c r="E47" s="44" t="s">
@@ -2466,13 +2475,13 @@
       <c r="J47" s="32"/>
     </row>
     <row r="48" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="49"/>
-      <c r="B48" s="52"/>
+      <c r="A48" s="52"/>
+      <c r="B48" s="54"/>
       <c r="C48" s="9">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-      <c r="D48" s="80" t="s">
+      <c r="D48" s="48" t="s">
         <v>78</v>
       </c>
       <c r="E48" s="44"/>
@@ -2485,7 +2494,7 @@
       <c r="J48" s="32"/>
     </row>
     <row r="49" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="49"/>
+      <c r="A49" s="52"/>
       <c r="B49" s="46" t="s">
         <v>25</v>
       </c>
@@ -2493,7 +2502,7 @@
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
-      <c r="D49" s="80" t="s">
+      <c r="D49" s="48" t="s">
         <v>81</v>
       </c>
       <c r="E49" s="44"/>
@@ -2504,6 +2513,9 @@
       <c r="H49" s="35"/>
       <c r="I49" s="33"/>
       <c r="J49" s="32"/>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D50" s="83"/>
     </row>
   </sheetData>
   <mergeCells count="30">

</xml_diff>

<commit_message>
[Criado] Art 16. - DFD Tratar empacotamento [Alteração] Art 16. - DFD Tratar Pedido, Art 17.
</commit_message>
<xml_diff>
--- a/Documentation/17-Analise_dos_Eventos_para_cada_Cenario.xlsx
+++ b/Documentation/17-Analise_dos_Eventos_para_cada_Cenario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/eed59d4ebf12600b/Documentos/Projeto/Faculdade/Silpan/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="378" documentId="8_{76FC5D5F-DBAD-408C-BCAE-F93491C61B30}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{FC9C34CB-46AE-4374-908D-145CEFBCA4C6}"/>
+  <xr:revisionPtr revIDLastSave="390" documentId="8_{76FC5D5F-DBAD-408C-BCAE-F93491C61B30}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{618A76F5-30A6-4C6B-904A-01823DCA1D1D}"/>
   <bookViews>
     <workbookView xWindow="-16320" yWindow="-8580" windowWidth="16440" windowHeight="38190" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="92">
   <si>
     <t>Capacidades</t>
   </si>
@@ -198,18 +198,12 @@
     <t>x(6, 10)</t>
   </si>
   <si>
-    <t>x(13)</t>
-  </si>
-  <si>
     <t>x(19)</t>
   </si>
   <si>
     <t>Vendedor entrega pedido</t>
   </si>
   <si>
-    <t>x(20)</t>
-  </si>
-  <si>
     <t>x(22)</t>
   </si>
   <si>
@@ -219,9 +213,6 @@
     <t>Vendedor efetiva pedido com orçamento</t>
   </si>
   <si>
-    <t>x(14)</t>
-  </si>
-  <si>
     <t>Tratar pagamento em dinheiro</t>
   </si>
   <si>
@@ -279,9 +270,6 @@
     <t>Caixa entrega comprovante de estorno</t>
   </si>
   <si>
-    <t>x(17)</t>
-  </si>
-  <si>
     <t>x(15, 18)</t>
   </si>
   <si>
@@ -358,6 +346,9 @@
   </si>
   <si>
     <t>x(44)</t>
+  </si>
+  <si>
+    <t>Vendedor solicita separação do pedido</t>
   </si>
 </sst>
 </file>
@@ -954,9 +945,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -993,16 +981,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1021,9 +1000,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1094,18 +1070,43 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1136,27 +1137,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1178,19 +1167,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1507,8 +1498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1521,56 +1512,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="63"/>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="55" t="s">
-        <v>73</v>
-      </c>
-      <c r="F1" s="56"/>
-      <c r="G1" s="59" t="s">
-        <v>74</v>
-      </c>
-      <c r="H1" s="60"/>
-      <c r="I1" s="61"/>
+      <c r="A1" s="67"/>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="59" t="s">
+        <v>69</v>
+      </c>
+      <c r="F1" s="60"/>
+      <c r="G1" s="63" t="s">
+        <v>70</v>
+      </c>
+      <c r="H1" s="64"/>
+      <c r="I1" s="65"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="64"/>
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="58"/>
-      <c r="G2" s="57"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="58"/>
-      <c r="J2" s="18"/>
+      <c r="A2" s="68"/>
+      <c r="B2" s="68"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="66"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="15"/>
     </row>
     <row r="3" spans="1:10" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="66" t="s">
+      <c r="A3" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="67"/>
-      <c r="C3" s="8" t="s">
+      <c r="B3" s="70"/>
+      <c r="C3" s="7" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="47" t="s">
+      <c r="E3" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="47" t="s">
+      <c r="F3" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="47" t="s">
+      <c r="G3" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="47" t="s">
+      <c r="H3" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="47" t="s">
+      <c r="I3" s="42" t="s">
         <v>7</v>
       </c>
       <c r="J3" s="2" t="s">
@@ -1578,121 +1569,121 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="16.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="50" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="68" t="s">
+      <c r="B4" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="8">
         <v>1</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5" t="s">
+      <c r="E4" s="4"/>
+      <c r="F4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="6"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10" ht="16.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="52"/>
-      <c r="B5" s="69"/>
-      <c r="C5" s="10">
+      <c r="A5" s="53"/>
+      <c r="B5" s="55"/>
+      <c r="C5" s="9">
         <f>C4+1</f>
         <v>2</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="4" t="s">
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="6"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10" ht="16.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="52"/>
-      <c r="B6" s="69"/>
-      <c r="C6" s="10">
+      <c r="A6" s="53"/>
+      <c r="B6" s="55"/>
+      <c r="C6" s="9">
         <f t="shared" ref="C6:C49" si="0">C5+1</f>
         <v>3</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="5"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="6"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10" ht="16.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="52"/>
-      <c r="B7" s="69"/>
-      <c r="C7" s="10">
+      <c r="A7" s="53"/>
+      <c r="B7" s="55"/>
+      <c r="C7" s="9">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="4" t="s">
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="6"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10" ht="16.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="52"/>
-      <c r="B8" s="69"/>
-      <c r="C8" s="10">
+      <c r="A8" s="53"/>
+      <c r="B8" s="55"/>
+      <c r="C8" s="9">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="5"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="6"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="16.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="71"/>
-      <c r="B9" s="70"/>
-      <c r="C9" s="10">
+      <c r="A9" s="51"/>
+      <c r="B9" s="71"/>
+      <c r="C9" s="9">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="4" t="s">
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="6"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="72" t="s">
@@ -1701,838 +1692,814 @@
       <c r="B10" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="9">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12" t="s">
+      <c r="E10" s="11"/>
+      <c r="F10" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="14"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="13"/>
     </row>
     <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="73"/>
       <c r="B11" s="76"/>
-      <c r="C11" s="10">
+      <c r="C11" s="9">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F11" s="5"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="6"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="73"/>
       <c r="B12" s="76"/>
-      <c r="C12" s="10">
+      <c r="C12" s="9">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="4" t="s">
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="6"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="73"/>
       <c r="B13" s="76"/>
-      <c r="C13" s="10">
+      <c r="C13" s="9">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="4" t="s">
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="6"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="74"/>
       <c r="B14" s="77" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="10">
+      <c r="C14" s="9">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="15" t="s">
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="J14" s="14"/>
+      <c r="J14" s="13"/>
     </row>
     <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="74"/>
       <c r="B15" s="78"/>
-      <c r="C15" s="24">
+      <c r="C15" s="20">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="D15" s="25" t="s">
+      <c r="D15" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="21" t="s">
+      <c r="E15" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="F15" s="21"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="22"/>
-      <c r="I15" s="22"/>
-      <c r="J15" s="23"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="19"/>
     </row>
     <row r="16" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="51" t="s">
+      <c r="A16" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="68" t="s">
+      <c r="B16" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="9">
+      <c r="C16" s="8">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="D16" s="26" t="s">
+      <c r="D16" s="79" t="s">
         <v>28</v>
       </c>
-      <c r="E16" s="27" t="s">
+      <c r="E16" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="F16" s="27"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="28"/>
-      <c r="I16" s="28"/>
-      <c r="J16" s="29"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="23"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="24"/>
     </row>
     <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="52"/>
-      <c r="B17" s="69"/>
-      <c r="C17" s="10">
+      <c r="A17" s="53"/>
+      <c r="B17" s="55"/>
+      <c r="C17" s="9">
         <f>C16+1</f>
         <v>14</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="4" t="s">
+      <c r="D17" s="80" t="s">
+        <v>45</v>
+      </c>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="25"/>
+    </row>
+    <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="53"/>
+      <c r="B18" s="55"/>
+      <c r="C18" s="9">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="D18" s="80" t="s">
+        <v>91</v>
+      </c>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="25"/>
+    </row>
+    <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="53"/>
+      <c r="B19" s="55"/>
+      <c r="C19" s="8">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="D19" s="81" t="s">
+        <v>42</v>
+      </c>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="25"/>
+    </row>
+    <row r="20" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="53"/>
+      <c r="B20" s="56" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="9">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="D20" s="82" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="25"/>
+    </row>
+    <row r="21" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="53"/>
+      <c r="B21" s="57"/>
+      <c r="C21" s="9">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="D21" s="83" t="s">
+        <v>44</v>
+      </c>
+      <c r="E21" s="16"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="26"/>
+    </row>
+    <row r="22" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="50" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" s="47" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="8">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="D22" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="E22" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="F22" s="31"/>
+      <c r="G22" s="29"/>
+      <c r="H22" s="29"/>
+      <c r="I22" s="28"/>
+      <c r="J22" s="27"/>
+    </row>
+    <row r="23" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="53"/>
+      <c r="B23" s="49"/>
+      <c r="C23" s="9">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="D23" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="E23" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="30"/>
-    </row>
-    <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="52"/>
-      <c r="B18" s="69"/>
-      <c r="C18" s="10">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="D18" s="3" t="s">
+      <c r="F23" s="32"/>
+      <c r="G23" s="30"/>
+      <c r="H23" s="30"/>
+      <c r="I23" s="29"/>
+      <c r="J23" s="33"/>
+    </row>
+    <row r="24" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="53"/>
+      <c r="B24" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="9">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="D24" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="E24" s="44"/>
+      <c r="F24" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G24" s="30"/>
+      <c r="H24" s="30"/>
+      <c r="I24" s="30"/>
+      <c r="J24" s="33"/>
+    </row>
+    <row r="25" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="50" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25" s="47" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" s="8">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="D25" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="4" t="s">
+      <c r="E25" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="F25" s="31"/>
+      <c r="G25" s="29"/>
+      <c r="H25" s="29"/>
+      <c r="I25" s="28"/>
+      <c r="J25" s="27"/>
+    </row>
+    <row r="26" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="53"/>
+      <c r="B26" s="49"/>
+      <c r="C26" s="9">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="D26" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="E26" s="39" t="s">
+        <v>43</v>
+      </c>
+      <c r="F26" s="32"/>
+      <c r="G26" s="30"/>
+      <c r="H26" s="30"/>
+      <c r="I26" s="29"/>
+      <c r="J26" s="33"/>
+    </row>
+    <row r="27" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="53"/>
+      <c r="B27" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27" s="9">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="D27" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="30"/>
-    </row>
-    <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="52"/>
-      <c r="B19" s="69"/>
-      <c r="C19" s="9">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="D19" s="16" t="s">
+      <c r="E27" s="44"/>
+      <c r="F27" s="45" t="s">
+        <v>11</v>
+      </c>
+      <c r="G27" s="30"/>
+      <c r="H27" s="30"/>
+      <c r="I27" s="30"/>
+      <c r="J27" s="33"/>
+    </row>
+    <row r="28" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="50" t="s">
+        <v>52</v>
+      </c>
+      <c r="B28" s="47" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" s="8">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="D28" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="E28" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="F28" s="31"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="29"/>
+      <c r="I28" s="28"/>
+      <c r="J28" s="27"/>
+    </row>
+    <row r="29" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="53"/>
+      <c r="B29" s="49"/>
+      <c r="C29" s="8">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="D29" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="E29" s="39" t="s">
+        <v>66</v>
+      </c>
+      <c r="F29" s="32"/>
+      <c r="G29" s="30"/>
+      <c r="H29" s="30"/>
+      <c r="I29" s="29"/>
+      <c r="J29" s="33"/>
+    </row>
+    <row r="30" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="53"/>
+      <c r="B30" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30" s="8">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="D30" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="E30" s="44"/>
+      <c r="F30" s="45" t="s">
+        <v>11</v>
+      </c>
+      <c r="G30" s="30"/>
+      <c r="H30" s="30"/>
+      <c r="I30" s="30"/>
+      <c r="J30" s="33"/>
+    </row>
+    <row r="31" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="50" t="s">
+        <v>54</v>
+      </c>
+      <c r="B31" s="47" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" s="8">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="D31" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="E31" s="38"/>
+      <c r="F31" s="31"/>
+      <c r="G31" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="H31" s="29"/>
+      <c r="I31" s="28"/>
+      <c r="J31" s="27"/>
+    </row>
+    <row r="32" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="53"/>
+      <c r="B32" s="48"/>
+      <c r="C32" s="8">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="D32" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="E32" s="39"/>
+      <c r="F32" s="32"/>
+      <c r="G32" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="H32" s="30"/>
+      <c r="I32" s="28"/>
+      <c r="J32" s="27"/>
+    </row>
+    <row r="33" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="53"/>
+      <c r="B33" s="49"/>
+      <c r="C33" s="8">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="D33" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="E33" s="39"/>
+      <c r="F33" s="32"/>
+      <c r="G33" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="H33" s="30"/>
+      <c r="I33" s="29"/>
+      <c r="J33" s="33"/>
+    </row>
+    <row r="34" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="50" t="s">
+        <v>55</v>
+      </c>
+      <c r="B34" s="47" t="s">
+        <v>9</v>
+      </c>
+      <c r="C34" s="8">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="D34" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="E34" s="38" t="s">
+        <v>80</v>
+      </c>
+      <c r="F34" s="31"/>
+      <c r="G34" s="29"/>
+      <c r="H34" s="29"/>
+      <c r="I34" s="28"/>
+      <c r="J34" s="27"/>
+    </row>
+    <row r="35" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="53"/>
+      <c r="B35" s="48"/>
+      <c r="C35" s="8">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="D35" s="36" t="s">
+        <v>59</v>
+      </c>
+      <c r="E35" s="39" t="s">
+        <v>81</v>
+      </c>
+      <c r="F35" s="32"/>
+      <c r="G35" s="30"/>
+      <c r="H35" s="30"/>
+      <c r="I35" s="28"/>
+      <c r="J35" s="27"/>
+    </row>
+    <row r="36" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="51"/>
+      <c r="B36" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="C36" s="8">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="D36" s="36" t="s">
+        <v>62</v>
+      </c>
+      <c r="E36" s="39"/>
+      <c r="F36" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="G36" s="30"/>
+      <c r="H36" s="30"/>
+      <c r="I36" s="28"/>
+      <c r="J36" s="27"/>
+    </row>
+    <row r="37" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="50" t="s">
+        <v>56</v>
+      </c>
+      <c r="B37" s="47" t="s">
+        <v>9</v>
+      </c>
+      <c r="C37" s="8">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="D37" s="36" t="s">
+        <v>58</v>
+      </c>
+      <c r="E37" s="38" t="s">
+        <v>80</v>
+      </c>
+      <c r="F37" s="32"/>
+      <c r="G37" s="30"/>
+      <c r="H37" s="30"/>
+      <c r="I37" s="29"/>
+      <c r="J37" s="33"/>
+    </row>
+    <row r="38" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="53"/>
+      <c r="B38" s="48"/>
+      <c r="C38" s="8">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="D38" s="36" t="s">
+        <v>59</v>
+      </c>
+      <c r="E38" s="38" t="s">
+        <v>82</v>
+      </c>
+      <c r="F38" s="32"/>
+      <c r="G38" s="30"/>
+      <c r="H38" s="30"/>
+      <c r="I38" s="28"/>
+      <c r="J38" s="27"/>
+    </row>
+    <row r="39" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="53"/>
+      <c r="B39" s="49"/>
+      <c r="C39" s="8">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="D39" s="36" t="s">
+        <v>61</v>
+      </c>
+      <c r="E39" s="38" t="s">
+        <v>83</v>
+      </c>
+      <c r="F39" s="32"/>
+      <c r="G39" s="30"/>
+      <c r="H39" s="30"/>
+      <c r="I39" s="29"/>
+      <c r="J39" s="33"/>
+    </row>
+    <row r="40" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="51"/>
+      <c r="B40" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="C40" s="8">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="D40" s="36" t="s">
+        <v>62</v>
+      </c>
+      <c r="E40" s="39"/>
+      <c r="F40" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="G40" s="30"/>
+      <c r="H40" s="30"/>
+      <c r="I40" s="30"/>
+      <c r="J40" s="33"/>
+    </row>
+    <row r="41" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="50" t="s">
+        <v>60</v>
+      </c>
+      <c r="B41" s="47" t="s">
+        <v>9</v>
+      </c>
+      <c r="C41" s="8">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="D41" s="35" t="s">
+        <v>63</v>
+      </c>
+      <c r="E41" s="38" t="s">
+        <v>84</v>
+      </c>
+      <c r="F41" s="31"/>
+      <c r="G41" s="29"/>
+      <c r="H41" s="29"/>
+      <c r="I41" s="28"/>
+      <c r="J41" s="27"/>
+    </row>
+    <row r="42" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="51"/>
+      <c r="B42" s="52"/>
+      <c r="C42" s="8">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="D42" s="36" t="s">
+        <v>64</v>
+      </c>
+      <c r="E42" s="39" t="s">
+        <v>85</v>
+      </c>
+      <c r="F42" s="32"/>
+      <c r="G42" s="30"/>
+      <c r="H42" s="30"/>
+      <c r="I42" s="28"/>
+      <c r="J42" s="27"/>
+    </row>
+    <row r="43" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="50" t="s">
+        <v>67</v>
+      </c>
+      <c r="B43" s="58" t="s">
+        <v>9</v>
+      </c>
+      <c r="C43" s="8">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="D43" s="43" t="s">
+        <v>71</v>
+      </c>
+      <c r="E43" s="39"/>
+      <c r="F43" s="32"/>
+      <c r="G43" s="30"/>
+      <c r="H43" s="30"/>
+      <c r="I43" s="28"/>
+      <c r="J43" s="27" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="53"/>
+      <c r="B44" s="48"/>
+      <c r="C44" s="8">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="D44" s="43" t="s">
+        <v>75</v>
+      </c>
+      <c r="E44" s="39" t="s">
+        <v>86</v>
+      </c>
+      <c r="F44" s="32"/>
+      <c r="G44" s="30"/>
+      <c r="H44" s="30"/>
+      <c r="I44" s="28"/>
+      <c r="J44" s="27"/>
+    </row>
+    <row r="45" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="53"/>
+      <c r="B45" s="48"/>
+      <c r="C45" s="8">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="D45" s="43" t="s">
+        <v>76</v>
+      </c>
+      <c r="E45" s="39"/>
+      <c r="F45" s="32"/>
+      <c r="G45" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="H45" s="30"/>
+      <c r="I45" s="28"/>
+      <c r="J45" s="27"/>
+    </row>
+    <row r="46" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="53"/>
+      <c r="B46" s="52"/>
+      <c r="C46" s="8">
+        <f t="shared" si="0"/>
         <v>43</v>
       </c>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="4" t="s">
+      <c r="D46" s="43" t="s">
+        <v>72</v>
+      </c>
+      <c r="E46" s="39"/>
+      <c r="F46" s="32"/>
+      <c r="G46" s="30" t="s">
+        <v>88</v>
+      </c>
+      <c r="H46" s="30"/>
+      <c r="I46" s="28"/>
+      <c r="J46" s="27"/>
+    </row>
+    <row r="47" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="50" t="s">
+        <v>68</v>
+      </c>
+      <c r="B47" s="58" t="s">
+        <v>9</v>
+      </c>
+      <c r="C47" s="8">
+        <f t="shared" si="0"/>
         <v>44</v>
       </c>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="30"/>
-    </row>
-    <row r="20" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="52"/>
-      <c r="B20" s="81" t="s">
+      <c r="D47" s="43" t="s">
+        <v>73</v>
+      </c>
+      <c r="E47" s="39" t="s">
+        <v>89</v>
+      </c>
+      <c r="F47" s="32"/>
+      <c r="G47" s="30"/>
+      <c r="H47" s="30"/>
+      <c r="I47" s="28"/>
+      <c r="J47" s="27"/>
+    </row>
+    <row r="48" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="53"/>
+      <c r="B48" s="52"/>
+      <c r="C48" s="8">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="D48" s="43" t="s">
+        <v>74</v>
+      </c>
+      <c r="E48" s="39"/>
+      <c r="F48" s="32"/>
+      <c r="G48" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="H48" s="30"/>
+      <c r="I48" s="28"/>
+      <c r="J48" s="27"/>
+    </row>
+    <row r="49" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="53"/>
+      <c r="B49" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="C20" s="10">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="D20" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5" t="s">
+      <c r="C49" s="8">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="D49" s="43" t="s">
+        <v>77</v>
+      </c>
+      <c r="E49" s="39"/>
+      <c r="F49" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="30"/>
-    </row>
-    <row r="21" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="52"/>
-      <c r="B21" s="82"/>
-      <c r="C21" s="10">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="D21" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="E21" s="20"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="H21" s="22"/>
-      <c r="I21" s="22"/>
-      <c r="J21" s="31"/>
-    </row>
-    <row r="22" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="51" t="s">
-        <v>49</v>
-      </c>
-      <c r="B22" s="79" t="s">
-        <v>9</v>
-      </c>
-      <c r="C22" s="9">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="D22" s="40" t="s">
-        <v>50</v>
-      </c>
-      <c r="E22" s="43" t="s">
-        <v>69</v>
-      </c>
-      <c r="F22" s="36"/>
-      <c r="G22" s="34"/>
-      <c r="H22" s="34"/>
-      <c r="I22" s="33"/>
-      <c r="J22" s="32"/>
-    </row>
-    <row r="23" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="52"/>
-      <c r="B23" s="80"/>
-      <c r="C23" s="10">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="D23" s="41" t="s">
-        <v>53</v>
-      </c>
-      <c r="E23" s="44" t="s">
-        <v>42</v>
-      </c>
-      <c r="F23" s="37"/>
-      <c r="G23" s="35"/>
-      <c r="H23" s="35"/>
-      <c r="I23" s="34"/>
-      <c r="J23" s="38"/>
-    </row>
-    <row r="24" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="52"/>
-      <c r="B24" s="39" t="s">
-        <v>25</v>
-      </c>
-      <c r="C24" s="10">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="D24" s="42" t="s">
-        <v>51</v>
-      </c>
-      <c r="E24" s="49"/>
-      <c r="F24" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G24" s="35"/>
-      <c r="H24" s="35"/>
-      <c r="I24" s="35"/>
-      <c r="J24" s="38"/>
-    </row>
-    <row r="25" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="51" t="s">
-        <v>52</v>
-      </c>
-      <c r="B25" s="79" t="s">
-        <v>9</v>
-      </c>
-      <c r="C25" s="9">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="D25" s="40" t="s">
-        <v>50</v>
-      </c>
-      <c r="E25" s="43" t="s">
-        <v>69</v>
-      </c>
-      <c r="F25" s="36"/>
-      <c r="G25" s="34"/>
-      <c r="H25" s="34"/>
-      <c r="I25" s="33"/>
-      <c r="J25" s="32"/>
-    </row>
-    <row r="26" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="52"/>
-      <c r="B26" s="80"/>
-      <c r="C26" s="10">
-        <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-      <c r="D26" s="41" t="s">
-        <v>54</v>
-      </c>
-      <c r="E26" s="44" t="s">
-        <v>45</v>
-      </c>
-      <c r="F26" s="37"/>
-      <c r="G26" s="35"/>
-      <c r="H26" s="35"/>
-      <c r="I26" s="34"/>
-      <c r="J26" s="38"/>
-    </row>
-    <row r="27" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="52"/>
-      <c r="B27" s="39" t="s">
-        <v>25</v>
-      </c>
-      <c r="C27" s="10">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="D27" s="42" t="s">
-        <v>51</v>
-      </c>
-      <c r="E27" s="49"/>
-      <c r="F27" s="50" t="s">
-        <v>11</v>
-      </c>
-      <c r="G27" s="35"/>
-      <c r="H27" s="35"/>
-      <c r="I27" s="35"/>
-      <c r="J27" s="38"/>
-    </row>
-    <row r="28" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="51" t="s">
-        <v>55</v>
-      </c>
-      <c r="B28" s="79" t="s">
-        <v>9</v>
-      </c>
-      <c r="C28" s="9">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="D28" s="40" t="s">
-        <v>50</v>
-      </c>
-      <c r="E28" s="43" t="s">
-        <v>69</v>
-      </c>
-      <c r="F28" s="36"/>
-      <c r="G28" s="34"/>
-      <c r="H28" s="34"/>
-      <c r="I28" s="33"/>
-      <c r="J28" s="32"/>
-    </row>
-    <row r="29" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="52"/>
-      <c r="B29" s="80"/>
-      <c r="C29" s="9">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-      <c r="D29" s="41" t="s">
-        <v>56</v>
-      </c>
-      <c r="E29" s="44" t="s">
-        <v>70</v>
-      </c>
-      <c r="F29" s="37"/>
-      <c r="G29" s="35"/>
-      <c r="H29" s="35"/>
-      <c r="I29" s="34"/>
-      <c r="J29" s="38"/>
-    </row>
-    <row r="30" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="52"/>
-      <c r="B30" s="39" t="s">
-        <v>25</v>
-      </c>
-      <c r="C30" s="9">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-      <c r="D30" s="42" t="s">
-        <v>51</v>
-      </c>
-      <c r="E30" s="49"/>
-      <c r="F30" s="50" t="s">
-        <v>11</v>
-      </c>
-      <c r="G30" s="35"/>
-      <c r="H30" s="35"/>
-      <c r="I30" s="35"/>
-      <c r="J30" s="38"/>
-    </row>
-    <row r="31" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="51" t="s">
-        <v>57</v>
-      </c>
-      <c r="B31" s="79" t="s">
-        <v>9</v>
-      </c>
-      <c r="C31" s="9">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-      <c r="D31" s="40" t="s">
-        <v>29</v>
-      </c>
-      <c r="E31" s="43"/>
-      <c r="F31" s="36"/>
-      <c r="G31" s="34" t="s">
-        <v>82</v>
-      </c>
-      <c r="H31" s="34"/>
-      <c r="I31" s="33"/>
-      <c r="J31" s="32"/>
-    </row>
-    <row r="32" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="52"/>
-      <c r="B32" s="65"/>
-      <c r="C32" s="9">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-      <c r="D32" s="41" t="s">
-        <v>30</v>
-      </c>
-      <c r="E32" s="44"/>
-      <c r="F32" s="37"/>
-      <c r="G32" s="35" t="s">
-        <v>83</v>
-      </c>
-      <c r="H32" s="35"/>
-      <c r="I32" s="33"/>
-      <c r="J32" s="32"/>
-    </row>
-    <row r="33" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="52"/>
-      <c r="B33" s="80"/>
-      <c r="C33" s="9">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="D33" s="41" t="s">
-        <v>31</v>
-      </c>
-      <c r="E33" s="44"/>
-      <c r="F33" s="37"/>
-      <c r="G33" s="35" t="s">
-        <v>84</v>
-      </c>
-      <c r="H33" s="35"/>
-      <c r="I33" s="34"/>
-      <c r="J33" s="38"/>
-    </row>
-    <row r="34" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="51" t="s">
-        <v>58</v>
-      </c>
-      <c r="B34" s="79" t="s">
-        <v>9</v>
-      </c>
-      <c r="C34" s="9">
-        <f t="shared" si="0"/>
-        <v>31</v>
-      </c>
-      <c r="D34" s="40" t="s">
-        <v>60</v>
-      </c>
-      <c r="E34" s="43" t="s">
-        <v>84</v>
-      </c>
-      <c r="F34" s="36"/>
-      <c r="G34" s="34"/>
-      <c r="H34" s="34"/>
-      <c r="I34" s="33"/>
-      <c r="J34" s="32"/>
-    </row>
-    <row r="35" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="52"/>
-      <c r="B35" s="65"/>
-      <c r="C35" s="9">
-        <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-      <c r="D35" s="41" t="s">
-        <v>62</v>
-      </c>
-      <c r="E35" s="44" t="s">
-        <v>85</v>
-      </c>
-      <c r="F35" s="37"/>
-      <c r="G35" s="35"/>
-      <c r="H35" s="35"/>
-      <c r="I35" s="33"/>
-      <c r="J35" s="32"/>
-    </row>
-    <row r="36" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="71"/>
-      <c r="B36" s="39" t="s">
-        <v>25</v>
-      </c>
-      <c r="C36" s="9">
-        <f t="shared" si="0"/>
-        <v>33</v>
-      </c>
-      <c r="D36" s="41" t="s">
-        <v>65</v>
-      </c>
-      <c r="E36" s="44"/>
-      <c r="F36" s="37" t="s">
-        <v>11</v>
-      </c>
-      <c r="G36" s="35"/>
-      <c r="H36" s="35"/>
-      <c r="I36" s="33"/>
-      <c r="J36" s="32"/>
-    </row>
-    <row r="37" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="51" t="s">
-        <v>59</v>
-      </c>
-      <c r="B37" s="79" t="s">
-        <v>9</v>
-      </c>
-      <c r="C37" s="9">
-        <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
-      <c r="D37" s="41" t="s">
-        <v>61</v>
-      </c>
-      <c r="E37" s="43" t="s">
-        <v>84</v>
-      </c>
-      <c r="F37" s="37"/>
-      <c r="G37" s="35"/>
-      <c r="H37" s="35"/>
-      <c r="I37" s="34"/>
-      <c r="J37" s="38"/>
-    </row>
-    <row r="38" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="52"/>
-      <c r="B38" s="65"/>
-      <c r="C38" s="9">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="D38" s="41" t="s">
-        <v>62</v>
-      </c>
-      <c r="E38" s="43" t="s">
-        <v>86</v>
-      </c>
-      <c r="F38" s="37"/>
-      <c r="G38" s="35"/>
-      <c r="H38" s="35"/>
-      <c r="I38" s="33"/>
-      <c r="J38" s="32"/>
-    </row>
-    <row r="39" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="52"/>
-      <c r="B39" s="80"/>
-      <c r="C39" s="9">
-        <f t="shared" si="0"/>
-        <v>36</v>
-      </c>
-      <c r="D39" s="41" t="s">
-        <v>64</v>
-      </c>
-      <c r="E39" s="43" t="s">
-        <v>87</v>
-      </c>
-      <c r="F39" s="37"/>
-      <c r="G39" s="35"/>
-      <c r="H39" s="35"/>
-      <c r="I39" s="34"/>
-      <c r="J39" s="38"/>
-    </row>
-    <row r="40" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="71"/>
-      <c r="B40" s="45" t="s">
-        <v>25</v>
-      </c>
-      <c r="C40" s="9">
-        <f t="shared" si="0"/>
-        <v>37</v>
-      </c>
-      <c r="D40" s="41" t="s">
-        <v>65</v>
-      </c>
-      <c r="E40" s="44"/>
-      <c r="F40" s="37" t="s">
-        <v>11</v>
-      </c>
-      <c r="G40" s="35"/>
-      <c r="H40" s="35"/>
-      <c r="I40" s="35"/>
-      <c r="J40" s="38"/>
-    </row>
-    <row r="41" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="51" t="s">
-        <v>63</v>
-      </c>
-      <c r="B41" s="79" t="s">
-        <v>9</v>
-      </c>
-      <c r="C41" s="9">
-        <f t="shared" si="0"/>
-        <v>38</v>
-      </c>
-      <c r="D41" s="40" t="s">
-        <v>66</v>
-      </c>
-      <c r="E41" s="43" t="s">
-        <v>88</v>
-      </c>
-      <c r="F41" s="36"/>
-      <c r="G41" s="34"/>
-      <c r="H41" s="34"/>
-      <c r="I41" s="33"/>
-      <c r="J41" s="32"/>
-    </row>
-    <row r="42" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="71"/>
-      <c r="B42" s="54"/>
-      <c r="C42" s="9">
-        <f t="shared" si="0"/>
-        <v>39</v>
-      </c>
-      <c r="D42" s="41" t="s">
-        <v>67</v>
-      </c>
-      <c r="E42" s="44" t="s">
-        <v>89</v>
-      </c>
-      <c r="F42" s="37"/>
-      <c r="G42" s="35"/>
-      <c r="H42" s="35"/>
-      <c r="I42" s="33"/>
-      <c r="J42" s="32"/>
-    </row>
-    <row r="43" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="51" t="s">
-        <v>71</v>
-      </c>
-      <c r="B43" s="53" t="s">
-        <v>9</v>
-      </c>
-      <c r="C43" s="9">
-        <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-      <c r="D43" s="48" t="s">
-        <v>75</v>
-      </c>
-      <c r="E43" s="44"/>
-      <c r="F43" s="37"/>
-      <c r="G43" s="35"/>
-      <c r="H43" s="35"/>
-      <c r="I43" s="33"/>
-      <c r="J43" s="32" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="52"/>
-      <c r="B44" s="65"/>
-      <c r="C44" s="9">
-        <f t="shared" si="0"/>
-        <v>41</v>
-      </c>
-      <c r="D44" s="48" t="s">
-        <v>79</v>
-      </c>
-      <c r="E44" s="44" t="s">
-        <v>90</v>
-      </c>
-      <c r="F44" s="37"/>
-      <c r="G44" s="35"/>
-      <c r="H44" s="35"/>
-      <c r="I44" s="33"/>
-      <c r="J44" s="32"/>
-    </row>
-    <row r="45" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="52"/>
-      <c r="B45" s="65"/>
-      <c r="C45" s="9">
-        <f t="shared" si="0"/>
-        <v>42</v>
-      </c>
-      <c r="D45" s="48" t="s">
-        <v>80</v>
-      </c>
-      <c r="E45" s="44"/>
-      <c r="F45" s="37"/>
-      <c r="G45" s="35" t="s">
-        <v>91</v>
-      </c>
-      <c r="H45" s="35"/>
-      <c r="I45" s="33"/>
-      <c r="J45" s="32"/>
-    </row>
-    <row r="46" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="52"/>
-      <c r="B46" s="54"/>
-      <c r="C46" s="9">
-        <f t="shared" si="0"/>
-        <v>43</v>
-      </c>
-      <c r="D46" s="48" t="s">
-        <v>76</v>
-      </c>
-      <c r="E46" s="44"/>
-      <c r="F46" s="37"/>
-      <c r="G46" s="35" t="s">
-        <v>92</v>
-      </c>
-      <c r="H46" s="35"/>
-      <c r="I46" s="33"/>
-      <c r="J46" s="32"/>
-    </row>
-    <row r="47" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="51" t="s">
-        <v>72</v>
-      </c>
-      <c r="B47" s="53" t="s">
-        <v>9</v>
-      </c>
-      <c r="C47" s="9">
-        <f t="shared" si="0"/>
-        <v>44</v>
-      </c>
-      <c r="D47" s="48" t="s">
-        <v>77</v>
-      </c>
-      <c r="E47" s="44" t="s">
-        <v>93</v>
-      </c>
-      <c r="F47" s="37"/>
-      <c r="G47" s="35"/>
-      <c r="H47" s="35"/>
-      <c r="I47" s="33"/>
-      <c r="J47" s="32"/>
-    </row>
-    <row r="48" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="52"/>
-      <c r="B48" s="54"/>
-      <c r="C48" s="9">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="D48" s="48" t="s">
-        <v>78</v>
-      </c>
-      <c r="E48" s="44"/>
-      <c r="F48" s="37"/>
-      <c r="G48" s="35" t="s">
-        <v>94</v>
-      </c>
-      <c r="H48" s="35"/>
-      <c r="I48" s="33"/>
-      <c r="J48" s="32"/>
-    </row>
-    <row r="49" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="52"/>
-      <c r="B49" s="46" t="s">
-        <v>25</v>
-      </c>
-      <c r="C49" s="9">
-        <f t="shared" si="0"/>
-        <v>46</v>
-      </c>
-      <c r="D49" s="48" t="s">
-        <v>81</v>
-      </c>
-      <c r="E49" s="44"/>
-      <c r="F49" s="37" t="s">
-        <v>11</v>
-      </c>
-      <c r="G49" s="35"/>
-      <c r="H49" s="35"/>
-      <c r="I49" s="33"/>
-      <c r="J49" s="32"/>
+      <c r="G49" s="30"/>
+      <c r="H49" s="30"/>
+      <c r="I49" s="28"/>
+      <c r="J49" s="27"/>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D50" s="83"/>
+      <c r="D50" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="B37:B39"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="A34:A36"/>
-    <mergeCell ref="A37:A40"/>
-    <mergeCell ref="B31:B33"/>
-    <mergeCell ref="B16:B19"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="A16:A21"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="A22:A24"/>
-    <mergeCell ref="A25:A27"/>
-    <mergeCell ref="B25:B26"/>
     <mergeCell ref="A47:A49"/>
     <mergeCell ref="B47:B48"/>
     <mergeCell ref="A43:A46"/>
@@ -2549,6 +2516,20 @@
     <mergeCell ref="A28:A30"/>
     <mergeCell ref="B28:B29"/>
     <mergeCell ref="A31:A33"/>
+    <mergeCell ref="B31:B33"/>
+    <mergeCell ref="B16:B19"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="A16:A21"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="B37:B39"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="A37:A40"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>